<commit_message>
Pre-monster fixes 2013, added score db save display error and retry. cleaned up display
</commit_message>
<xml_diff>
--- a/monster2013/Monster All.xlsx
+++ b/monster2013/Monster All.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="15240"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="15240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Monster" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="413">
   <si>
     <t>Total</t>
   </si>
@@ -1239,6 +1239,24 @@
   </si>
   <si>
     <t>Revenue</t>
+  </si>
+  <si>
+    <t>HR Team</t>
+  </si>
+  <si>
+    <t>HR Hole</t>
+  </si>
+  <si>
+    <t>HR Flight 1</t>
+  </si>
+  <si>
+    <t>HR Flight 2</t>
+  </si>
+  <si>
+    <t>HR Flight 3</t>
+  </si>
+  <si>
+    <t>HR Flight 4</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1369,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1447,6 +1465,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1495,7 +1519,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1698,6 +1722,27 @@
     <xf numFmtId="44" fontId="13" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="18" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1712,10 +1757,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1724,16 +1769,10 @@
     <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2044,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T28" sqref="T28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2167,7 +2206,7 @@
     </row>
     <row r="3" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="43"/>
-      <c r="B3" s="93">
+      <c r="B3" s="100">
         <v>0.40277777777777773</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -2177,10 +2216,10 @@
         <v>286</v>
       </c>
       <c r="E3" s="43"/>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="102" t="s">
         <v>315</v>
       </c>
-      <c r="G3" s="95">
+      <c r="G3" s="102">
         <v>1</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -2189,7 +2228,7 @@
       <c r="I3" s="31">
         <v>8</v>
       </c>
-      <c r="J3" s="95">
+      <c r="J3" s="102">
         <v>1</v>
       </c>
       <c r="K3" s="9" t="s">
@@ -2199,10 +2238,10 @@
         <v>16</v>
       </c>
       <c r="M3" s="10"/>
-      <c r="N3" s="95" t="s">
+      <c r="N3" s="102" t="s">
         <v>369</v>
       </c>
-      <c r="O3" s="95">
+      <c r="O3" s="102">
         <v>1</v>
       </c>
       <c r="P3" s="9" t="s">
@@ -2211,7 +2250,7 @@
       <c r="Q3" s="31">
         <v>8</v>
       </c>
-      <c r="R3" s="95">
+      <c r="R3" s="102">
         <v>1</v>
       </c>
       <c r="S3" s="9" t="s">
@@ -2224,7 +2263,7 @@
     </row>
     <row r="4" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="43"/>
-      <c r="B4" s="93"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="9" t="s">
         <v>60</v>
       </c>
@@ -2232,15 +2271,15 @@
         <v>62</v>
       </c>
       <c r="E4" s="43"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
       <c r="H4" s="12" t="s">
         <v>256</v>
       </c>
       <c r="I4" s="34">
         <v>2</v>
       </c>
-      <c r="J4" s="95"/>
+      <c r="J4" s="102"/>
       <c r="K4" s="13" t="s">
         <v>260</v>
       </c>
@@ -2248,15 +2287,15 @@
         <v>7</v>
       </c>
       <c r="M4" s="14"/>
-      <c r="N4" s="95"/>
-      <c r="O4" s="95"/>
+      <c r="N4" s="102"/>
+      <c r="O4" s="102"/>
       <c r="P4" s="12" t="s">
         <v>256</v>
       </c>
       <c r="Q4" s="34">
         <v>2</v>
       </c>
-      <c r="R4" s="95"/>
+      <c r="R4" s="102"/>
       <c r="S4" s="13" t="s">
         <v>258</v>
       </c>
@@ -2267,7 +2306,7 @@
     </row>
     <row r="5" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="43"/>
-      <c r="B5" s="94">
+      <c r="B5" s="101">
         <v>0.40972222222222227</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -2277,10 +2316,10 @@
         <v>57</v>
       </c>
       <c r="E5" s="43"/>
-      <c r="F5" s="96" t="s">
+      <c r="F5" s="103" t="s">
         <v>316</v>
       </c>
-      <c r="G5" s="96">
+      <c r="G5" s="103">
         <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -2289,7 +2328,7 @@
       <c r="I5" s="33">
         <v>5</v>
       </c>
-      <c r="J5" s="96">
+      <c r="J5" s="103">
         <v>1</v>
       </c>
       <c r="K5" s="3" t="s">
@@ -2299,10 +2338,10 @@
         <v>2</v>
       </c>
       <c r="M5" s="14"/>
-      <c r="N5" s="96" t="s">
+      <c r="N5" s="103" t="s">
         <v>368</v>
       </c>
-      <c r="O5" s="96">
+      <c r="O5" s="103">
         <v>1</v>
       </c>
       <c r="P5" s="3" t="s">
@@ -2311,7 +2350,7 @@
       <c r="Q5" s="33">
         <v>5</v>
       </c>
-      <c r="R5" s="96">
+      <c r="R5" s="103">
         <v>2</v>
       </c>
       <c r="S5" s="3" t="s">
@@ -2324,7 +2363,7 @@
     </row>
     <row r="6" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="43"/>
-      <c r="B6" s="94">
+      <c r="B6" s="101">
         <v>0.40972222222222227</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -2334,15 +2373,15 @@
         <v>58</v>
       </c>
       <c r="E6" s="43"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
       <c r="H6" s="3" t="s">
         <v>262</v>
       </c>
       <c r="I6" s="33">
         <v>12</v>
       </c>
-      <c r="J6" s="96"/>
+      <c r="J6" s="103"/>
       <c r="K6" s="3" t="s">
         <v>264</v>
       </c>
@@ -2350,15 +2389,15 @@
         <v>9</v>
       </c>
       <c r="M6" s="14"/>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="103"/>
       <c r="P6" s="3" t="s">
         <v>262</v>
       </c>
       <c r="Q6" s="33">
         <v>12</v>
       </c>
-      <c r="R6" s="96"/>
+      <c r="R6" s="103"/>
       <c r="S6" s="3" t="s">
         <v>270</v>
       </c>
@@ -2369,7 +2408,7 @@
     </row>
     <row r="7" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="43"/>
-      <c r="B7" s="93">
+      <c r="B7" s="100">
         <v>0.41666666666666669</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -2379,11 +2418,11 @@
         <v>33</v>
       </c>
       <c r="E7" s="43"/>
-      <c r="F7" s="95" t="s">
+      <c r="F7" s="102" t="s">
         <v>317</v>
       </c>
-      <c r="G7" s="95">
-        <v>3</v>
+      <c r="G7" s="102">
+        <v>2</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>266</v>
@@ -2391,7 +2430,7 @@
       <c r="I7" s="31">
         <v>22</v>
       </c>
-      <c r="J7" s="95">
+      <c r="J7" s="102">
         <v>1</v>
       </c>
       <c r="K7" s="9" t="s">
@@ -2401,10 +2440,10 @@
         <v>6</v>
       </c>
       <c r="M7" s="14"/>
-      <c r="N7" s="95" t="s">
+      <c r="N7" s="102" t="s">
         <v>317</v>
       </c>
-      <c r="O7" s="95">
+      <c r="O7" s="102">
         <v>1</v>
       </c>
       <c r="P7" s="9" t="s">
@@ -2413,7 +2452,7 @@
       <c r="Q7" s="31">
         <v>2</v>
       </c>
-      <c r="R7" s="95">
+      <c r="R7" s="102">
         <v>1</v>
       </c>
       <c r="S7" s="9" t="s">
@@ -2426,7 +2465,7 @@
     </row>
     <row r="8" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="43"/>
-      <c r="B8" s="93">
+      <c r="B8" s="100">
         <v>0.41666666666666669</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -2436,15 +2475,15 @@
         <v>34</v>
       </c>
       <c r="E8" s="43"/>
-      <c r="F8" s="95"/>
-      <c r="G8" s="95"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
       <c r="H8" s="9" t="s">
         <v>267</v>
       </c>
       <c r="I8" s="31">
-        <v>14</v>
-      </c>
-      <c r="J8" s="95"/>
+        <v>13</v>
+      </c>
+      <c r="J8" s="102"/>
       <c r="K8" s="9" t="s">
         <v>269</v>
       </c>
@@ -2452,15 +2491,15 @@
         <v>10</v>
       </c>
       <c r="M8" s="14"/>
-      <c r="N8" s="95"/>
-      <c r="O8" s="95"/>
+      <c r="N8" s="102"/>
+      <c r="O8" s="102"/>
       <c r="P8" s="9" t="s">
         <v>264</v>
       </c>
       <c r="Q8" s="31">
         <v>9</v>
       </c>
-      <c r="R8" s="95"/>
+      <c r="R8" s="102"/>
       <c r="S8" s="9" t="s">
         <v>276</v>
       </c>
@@ -2471,20 +2510,20 @@
     </row>
     <row r="9" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="43"/>
-      <c r="B9" s="94">
+      <c r="B9" s="101">
         <v>0.4236111111111111</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="E9" s="43"/>
-      <c r="F9" s="96" t="s">
+      <c r="F9" s="103" t="s">
         <v>327</v>
       </c>
-      <c r="G9" s="96">
+      <c r="G9" s="103">
         <v>1</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -2493,7 +2532,7 @@
       <c r="I9" s="33">
         <v>2</v>
       </c>
-      <c r="J9" s="96">
+      <c r="J9" s="103">
         <v>3</v>
       </c>
       <c r="K9" s="3" t="s">
@@ -2503,10 +2542,10 @@
         <v>22</v>
       </c>
       <c r="M9" s="14"/>
-      <c r="N9" s="96" t="s">
+      <c r="N9" s="103" t="s">
         <v>327</v>
       </c>
-      <c r="O9" s="96">
+      <c r="O9" s="103">
         <v>1</v>
       </c>
       <c r="P9" s="3" t="s">
@@ -2515,7 +2554,7 @@
       <c r="Q9" s="33">
         <v>16</v>
       </c>
-      <c r="R9" s="96">
+      <c r="R9" s="103">
         <v>2</v>
       </c>
       <c r="S9" s="3" t="s">
@@ -2528,25 +2567,23 @@
     </row>
     <row r="10" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="43"/>
-      <c r="B10" s="94">
-        <v>0.4236111111111111</v>
-      </c>
+      <c r="B10" s="101"/>
       <c r="C10" s="3" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="E10" s="43"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="103"/>
       <c r="H10" s="3" t="s">
         <v>258</v>
       </c>
       <c r="I10" s="33">
         <v>5</v>
       </c>
-      <c r="J10" s="96"/>
+      <c r="J10" s="103"/>
       <c r="K10" s="3" t="s">
         <v>272</v>
       </c>
@@ -2554,15 +2591,15 @@
         <v>24</v>
       </c>
       <c r="M10" s="14"/>
-      <c r="N10" s="96"/>
-      <c r="O10" s="96"/>
+      <c r="N10" s="103"/>
+      <c r="O10" s="103"/>
       <c r="P10" s="3" t="s">
         <v>259</v>
       </c>
       <c r="Q10" s="33">
         <v>7</v>
       </c>
-      <c r="R10" s="96"/>
+      <c r="R10" s="103"/>
       <c r="S10" s="3" t="s">
         <v>282</v>
       </c>
@@ -2573,20 +2610,20 @@
     </row>
     <row r="11" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="43"/>
-      <c r="B11" s="93">
+      <c r="B11" s="100">
         <v>0.43055555555555558</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>263</v>
+        <v>35</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E11" s="43"/>
-      <c r="F11" s="95" t="s">
+      <c r="F11" s="102" t="s">
         <v>336</v>
       </c>
-      <c r="G11" s="95">
+      <c r="G11" s="102">
         <v>1</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -2595,7 +2632,7 @@
       <c r="I11" s="31">
         <v>0</v>
       </c>
-      <c r="J11" s="95">
+      <c r="J11" s="102">
         <v>2</v>
       </c>
       <c r="K11" s="9" t="s">
@@ -2605,10 +2642,10 @@
         <v>8</v>
       </c>
       <c r="M11" s="14"/>
-      <c r="N11" s="95" t="s">
+      <c r="N11" s="102" t="s">
         <v>318</v>
       </c>
-      <c r="O11" s="95">
+      <c r="O11" s="102">
         <v>3</v>
       </c>
       <c r="P11" s="9" t="s">
@@ -2617,7 +2654,7 @@
       <c r="Q11" s="31">
         <v>22</v>
       </c>
-      <c r="R11" s="95">
+      <c r="R11" s="102">
         <v>1</v>
       </c>
       <c r="S11" s="9" t="s">
@@ -2630,23 +2667,25 @@
     </row>
     <row r="12" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="43"/>
-      <c r="B12" s="93">
-        <v>0.43055555555555558</v>
+      <c r="B12" s="100">
+        <v>0.4236111111111111</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="D12" s="9"/>
+        <v>43</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="E12" s="43"/>
-      <c r="F12" s="95"/>
-      <c r="G12" s="95"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
       <c r="H12" s="9" t="s">
         <v>276</v>
       </c>
       <c r="I12" s="31">
         <v>3</v>
       </c>
-      <c r="J12" s="95"/>
+      <c r="J12" s="102"/>
       <c r="K12" s="9" t="s">
         <v>270</v>
       </c>
@@ -2654,15 +2693,15 @@
         <v>20</v>
       </c>
       <c r="M12" s="14"/>
-      <c r="N12" s="95"/>
-      <c r="O12" s="95"/>
+      <c r="N12" s="102"/>
+      <c r="O12" s="102"/>
       <c r="P12" s="9" t="s">
         <v>272</v>
       </c>
       <c r="Q12" s="31">
         <v>24</v>
       </c>
-      <c r="R12" s="95"/>
+      <c r="R12" s="102"/>
       <c r="S12" s="9" t="s">
         <v>269</v>
       </c>
@@ -2673,20 +2712,20 @@
     </row>
     <row r="13" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="43"/>
-      <c r="B13" s="94">
+      <c r="B13" s="101">
         <v>0.4375</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>263</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>340</v>
+        <v>44</v>
       </c>
       <c r="E13" s="43"/>
-      <c r="F13" s="96" t="s">
+      <c r="F13" s="103" t="s">
         <v>360</v>
       </c>
-      <c r="G13" s="96">
+      <c r="G13" s="103">
         <v>1</v>
       </c>
       <c r="H13" s="15" t="s">
@@ -2695,7 +2734,7 @@
       <c r="I13" s="33">
         <v>8</v>
       </c>
-      <c r="J13" s="96">
+      <c r="J13" s="103">
         <v>2</v>
       </c>
       <c r="K13" s="15" t="s">
@@ -2705,10 +2744,10 @@
         <v>13</v>
       </c>
       <c r="M13" s="14"/>
-      <c r="N13" s="96" t="s">
+      <c r="N13" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="O13" s="96">
+      <c r="O13" s="103">
         <v>1</v>
       </c>
       <c r="P13" s="15" t="s">
@@ -2717,7 +2756,7 @@
       <c r="Q13" s="33">
         <v>8</v>
       </c>
-      <c r="R13" s="96">
+      <c r="R13" s="103">
         <v>3</v>
       </c>
       <c r="S13" s="15" t="s">
@@ -2730,23 +2769,23 @@
     </row>
     <row r="14" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="43"/>
-      <c r="B14" s="94"/>
+      <c r="B14" s="101">
+        <v>0.43055555555555558</v>
+      </c>
       <c r="C14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>342</v>
-      </c>
+        <v>352</v>
+      </c>
+      <c r="D14" s="3"/>
       <c r="E14" s="43"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="103"/>
       <c r="H14" s="3" t="s">
         <v>278</v>
       </c>
       <c r="I14" s="33">
         <v>12</v>
       </c>
-      <c r="J14" s="96"/>
+      <c r="J14" s="103"/>
       <c r="K14" s="3" t="s">
         <v>282</v>
       </c>
@@ -2754,15 +2793,15 @@
         <v>13</v>
       </c>
       <c r="M14" s="14"/>
-      <c r="N14" s="96"/>
-      <c r="O14" s="96"/>
+      <c r="N14" s="103"/>
+      <c r="O14" s="103"/>
       <c r="P14" s="3" t="s">
         <v>278</v>
       </c>
       <c r="Q14" s="33">
         <v>12</v>
       </c>
-      <c r="R14" s="96"/>
+      <c r="R14" s="103"/>
       <c r="S14" s="3" t="s">
         <v>274</v>
       </c>
@@ -2773,20 +2812,20 @@
     </row>
     <row r="15" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="43"/>
-      <c r="B15" s="93">
+      <c r="B15" s="100">
         <v>0.44444444444444442</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>21</v>
+        <v>340</v>
       </c>
       <c r="E15" s="43"/>
-      <c r="F15" s="95" t="s">
+      <c r="F15" s="102" t="s">
         <v>328</v>
       </c>
-      <c r="G15" s="95">
+      <c r="G15" s="102">
         <v>2</v>
       </c>
       <c r="H15" s="9" t="s">
@@ -2795,7 +2834,7 @@
       <c r="I15" s="31">
         <v>11</v>
       </c>
-      <c r="J15" s="95">
+      <c r="J15" s="102">
         <v>2</v>
       </c>
       <c r="K15" s="9" t="s">
@@ -2805,11 +2844,11 @@
         <v>15</v>
       </c>
       <c r="M15" s="14"/>
-      <c r="N15" s="95" t="s">
+      <c r="N15" s="102" t="s">
         <v>319</v>
       </c>
-      <c r="O15" s="95">
-        <v>3</v>
+      <c r="O15" s="102">
+        <v>2</v>
       </c>
       <c r="P15" s="9" t="s">
         <v>266</v>
@@ -2817,7 +2856,7 @@
       <c r="Q15" s="31">
         <v>22</v>
       </c>
-      <c r="R15" s="95">
+      <c r="R15" s="102">
         <v>2</v>
       </c>
       <c r="S15" s="9" t="s">
@@ -2830,21 +2869,23 @@
     </row>
     <row r="16" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="43"/>
-      <c r="B16" s="93"/>
+      <c r="B16" s="100"/>
       <c r="C16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="9"/>
+        <v>52</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>342</v>
+      </c>
       <c r="E16" s="43"/>
-      <c r="F16" s="95"/>
-      <c r="G16" s="95"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="102"/>
       <c r="H16" s="9" t="s">
         <v>286</v>
       </c>
       <c r="I16" s="31">
         <v>18</v>
       </c>
-      <c r="J16" s="95"/>
+      <c r="J16" s="102"/>
       <c r="K16" s="9" t="s">
         <v>280</v>
       </c>
@@ -2852,15 +2893,15 @@
         <v>17</v>
       </c>
       <c r="M16" s="14"/>
-      <c r="N16" s="95"/>
-      <c r="O16" s="95"/>
+      <c r="N16" s="102"/>
+      <c r="O16" s="102"/>
       <c r="P16" s="9" t="s">
         <v>267</v>
       </c>
       <c r="Q16" s="31">
-        <v>14</v>
-      </c>
-      <c r="R16" s="95"/>
+        <v>13</v>
+      </c>
+      <c r="R16" s="102"/>
       <c r="S16" s="9" t="s">
         <v>284</v>
       </c>
@@ -2871,20 +2912,20 @@
     </row>
     <row r="17" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="43"/>
-      <c r="B17" s="94">
+      <c r="B17" s="101">
         <v>0.4513888888888889</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="E17" s="43"/>
-      <c r="F17" s="96" t="s">
+      <c r="F17" s="103" t="s">
         <v>337</v>
       </c>
-      <c r="G17" s="96">
+      <c r="G17" s="103">
         <v>3</v>
       </c>
       <c r="H17" s="3" t="s">
@@ -2893,7 +2934,7 @@
       <c r="I17" s="33">
         <v>23</v>
       </c>
-      <c r="J17" s="96">
+      <c r="J17" s="103">
         <v>2</v>
       </c>
       <c r="K17" s="3" t="s">
@@ -2903,10 +2944,10 @@
         <v>12</v>
       </c>
       <c r="M17" s="14"/>
-      <c r="N17" s="96" t="s">
+      <c r="N17" s="103" t="s">
         <v>329</v>
       </c>
-      <c r="O17" s="96">
+      <c r="O17" s="103">
         <v>2</v>
       </c>
       <c r="P17" s="3" t="s">
@@ -2915,7 +2956,7 @@
       <c r="Q17" s="33">
         <v>12</v>
       </c>
-      <c r="R17" s="96">
+      <c r="R17" s="103">
         <v>2</v>
       </c>
       <c r="S17" s="3" t="s">
@@ -2928,23 +2969,21 @@
     </row>
     <row r="18" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="43"/>
-      <c r="B18" s="94"/>
+      <c r="B18" s="101"/>
       <c r="C18" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>68</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D18" s="3"/>
       <c r="E18" s="43"/>
-      <c r="F18" s="96"/>
-      <c r="G18" s="96"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="103"/>
       <c r="H18" s="3" t="s">
         <v>288</v>
       </c>
       <c r="I18" s="33">
         <v>19</v>
       </c>
-      <c r="J18" s="96"/>
+      <c r="J18" s="103"/>
       <c r="K18" s="3" t="s">
         <v>290</v>
       </c>
@@ -2952,15 +2991,15 @@
         <v>22</v>
       </c>
       <c r="M18" s="14"/>
-      <c r="N18" s="96"/>
-      <c r="O18" s="96"/>
+      <c r="N18" s="103"/>
+      <c r="O18" s="103"/>
       <c r="P18" s="3" t="s">
         <v>290</v>
       </c>
       <c r="Q18" s="33">
         <v>22</v>
       </c>
-      <c r="R18" s="96"/>
+      <c r="R18" s="103"/>
       <c r="S18" s="3" t="s">
         <v>280</v>
       </c>
@@ -2971,7 +3010,7 @@
     </row>
     <row r="19" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="43"/>
-      <c r="B19" s="93">
+      <c r="B19" s="100">
         <v>0.45833333333333331</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -2981,10 +3020,10 @@
         <v>56</v>
       </c>
       <c r="E19" s="43"/>
-      <c r="F19" s="95" t="s">
+      <c r="F19" s="102" t="s">
         <v>338</v>
       </c>
-      <c r="G19" s="95">
+      <c r="G19" s="102">
         <v>1</v>
       </c>
       <c r="H19" s="9" t="s">
@@ -2993,7 +3032,7 @@
       <c r="I19" s="31">
         <v>12</v>
       </c>
-      <c r="J19" s="95">
+      <c r="J19" s="102">
         <v>3</v>
       </c>
       <c r="K19" s="9" t="s">
@@ -3003,10 +3042,10 @@
         <v>21</v>
       </c>
       <c r="M19" s="16"/>
-      <c r="N19" s="95" t="s">
+      <c r="N19" s="102" t="s">
         <v>322</v>
       </c>
-      <c r="O19" s="95">
+      <c r="O19" s="102">
         <v>1</v>
       </c>
       <c r="P19" s="9" t="s">
@@ -3015,7 +3054,7 @@
       <c r="Q19" s="31">
         <v>12</v>
       </c>
-      <c r="R19" s="95">
+      <c r="R19" s="102">
         <v>2</v>
       </c>
       <c r="S19" s="9" t="s">
@@ -3028,7 +3067,7 @@
     </row>
     <row r="20" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="43"/>
-      <c r="B20" s="93"/>
+      <c r="B20" s="100"/>
       <c r="C20" s="9" t="s">
         <v>308</v>
       </c>
@@ -3036,15 +3075,15 @@
         <v>64</v>
       </c>
       <c r="E20" s="43"/>
-      <c r="F20" s="95"/>
-      <c r="G20" s="95"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="102"/>
       <c r="H20" s="9" t="s">
         <v>96</v>
       </c>
       <c r="I20" s="31">
         <v>6</v>
       </c>
-      <c r="J20" s="95"/>
+      <c r="J20" s="102"/>
       <c r="K20" s="9" t="s">
         <v>310</v>
       </c>
@@ -3052,15 +3091,15 @@
         <v>31</v>
       </c>
       <c r="M20" s="14"/>
-      <c r="N20" s="95"/>
-      <c r="O20" s="95"/>
+      <c r="N20" s="102"/>
+      <c r="O20" s="102"/>
       <c r="P20" s="9" t="s">
         <v>96</v>
       </c>
       <c r="Q20" s="31">
         <v>6</v>
       </c>
-      <c r="R20" s="95"/>
+      <c r="R20" s="102"/>
       <c r="S20" s="9" t="s">
         <v>298</v>
       </c>
@@ -3071,7 +3110,7 @@
     </row>
     <row r="21" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="43"/>
-      <c r="B21" s="94">
+      <c r="B21" s="101">
         <v>0.46527777777777773</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -3081,10 +3120,10 @@
         <v>134</v>
       </c>
       <c r="E21" s="43"/>
-      <c r="F21" s="96" t="s">
+      <c r="F21" s="103" t="s">
         <v>320</v>
       </c>
-      <c r="G21" s="96">
+      <c r="G21" s="103">
         <v>1</v>
       </c>
       <c r="H21" s="3" t="s">
@@ -3093,7 +3132,7 @@
       <c r="I21" s="33">
         <v>14</v>
       </c>
-      <c r="J21" s="96">
+      <c r="J21" s="103">
         <v>2</v>
       </c>
       <c r="K21" s="3" t="s">
@@ -3103,11 +3142,11 @@
         <v>12</v>
       </c>
       <c r="M21" s="14"/>
-      <c r="N21" s="96" t="s">
+      <c r="N21" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="O21" s="96">
-        <v>2</v>
+      <c r="O21" s="103">
+        <v>3</v>
       </c>
       <c r="P21" s="3" t="s">
         <v>301</v>
@@ -3115,7 +3154,7 @@
       <c r="Q21" s="33">
         <v>21</v>
       </c>
-      <c r="R21" s="96">
+      <c r="R21" s="103">
         <v>2</v>
       </c>
       <c r="S21" s="3" t="s">
@@ -3128,7 +3167,7 @@
     </row>
     <row r="22" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="43"/>
-      <c r="B22" s="94"/>
+      <c r="B22" s="101"/>
       <c r="C22" s="3" t="s">
         <v>40</v>
       </c>
@@ -3136,15 +3175,15 @@
         <v>135</v>
       </c>
       <c r="E22" s="43"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
+      <c r="F22" s="103"/>
+      <c r="G22" s="103"/>
       <c r="H22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I22" s="33">
         <v>7</v>
       </c>
-      <c r="J22" s="96"/>
+      <c r="J22" s="103"/>
       <c r="K22" s="3" t="s">
         <v>284</v>
       </c>
@@ -3152,15 +3191,15 @@
         <v>13</v>
       </c>
       <c r="M22" s="14"/>
-      <c r="N22" s="96"/>
-      <c r="O22" s="96"/>
+      <c r="N22" s="103"/>
+      <c r="O22" s="103"/>
       <c r="P22" s="3" t="s">
         <v>302</v>
       </c>
       <c r="Q22" s="33">
         <v>14</v>
       </c>
-      <c r="R22" s="96"/>
+      <c r="R22" s="103"/>
       <c r="S22" s="3" t="s">
         <v>286</v>
       </c>
@@ -3171,7 +3210,7 @@
     </row>
     <row r="23" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="43"/>
-      <c r="B23" s="93">
+      <c r="B23" s="100">
         <v>0.47916666666666669</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -3181,10 +3220,10 @@
         <v>353</v>
       </c>
       <c r="E23" s="43"/>
-      <c r="F23" s="95" t="s">
+      <c r="F23" s="102" t="s">
         <v>321</v>
       </c>
-      <c r="G23" s="95">
+      <c r="G23" s="102">
         <v>2</v>
       </c>
       <c r="H23" s="9" t="s">
@@ -3193,7 +3232,7 @@
       <c r="I23" s="31">
         <v>18</v>
       </c>
-      <c r="J23" s="95">
+      <c r="J23" s="102">
         <v>3</v>
       </c>
       <c r="K23" s="9" t="s">
@@ -3203,10 +3242,10 @@
         <v>27</v>
       </c>
       <c r="M23" s="14"/>
-      <c r="N23" s="95" t="s">
+      <c r="N23" s="102" t="s">
         <v>324</v>
       </c>
-      <c r="O23" s="95">
+      <c r="O23" s="102">
         <v>1</v>
       </c>
       <c r="P23" s="9" t="s">
@@ -3215,7 +3254,7 @@
       <c r="Q23" s="31">
         <v>10</v>
       </c>
-      <c r="R23" s="95">
+      <c r="R23" s="102">
         <v>3</v>
       </c>
       <c r="S23" s="9" t="s">
@@ -3228,7 +3267,7 @@
     </row>
     <row r="24" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="43"/>
-      <c r="B24" s="93"/>
+      <c r="B24" s="100"/>
       <c r="C24" s="9" t="s">
         <v>50</v>
       </c>
@@ -3236,15 +3275,15 @@
         <v>354</v>
       </c>
       <c r="E24" s="43"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="95"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="102"/>
       <c r="H24" s="9" t="s">
         <v>300</v>
       </c>
       <c r="I24" s="31">
         <v>14</v>
       </c>
-      <c r="J24" s="95"/>
+      <c r="J24" s="102"/>
       <c r="K24" s="9" t="s">
         <v>305</v>
       </c>
@@ -3252,15 +3291,15 @@
         <v>15</v>
       </c>
       <c r="M24" s="14"/>
-      <c r="N24" s="95"/>
-      <c r="O24" s="95"/>
+      <c r="N24" s="102"/>
+      <c r="O24" s="102"/>
       <c r="P24" s="9" t="s">
         <v>293</v>
       </c>
       <c r="Q24" s="31">
         <v>14</v>
       </c>
-      <c r="R24" s="95"/>
+      <c r="R24" s="102"/>
       <c r="S24" s="9" t="s">
         <v>305</v>
       </c>
@@ -3271,7 +3310,7 @@
     </row>
     <row r="25" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="43"/>
-      <c r="B25" s="94">
+      <c r="B25" s="101">
         <v>0.4861111111111111</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -3281,10 +3320,10 @@
         <v>24</v>
       </c>
       <c r="E25" s="43"/>
-      <c r="F25" s="96" t="s">
+      <c r="F25" s="103" t="s">
         <v>359</v>
       </c>
-      <c r="G25" s="96">
+      <c r="G25" s="103">
         <v>2</v>
       </c>
       <c r="H25" s="3" t="s">
@@ -3293,7 +3332,7 @@
       <c r="I25" s="33">
         <v>11</v>
       </c>
-      <c r="J25" s="96">
+      <c r="J25" s="103">
         <v>3</v>
       </c>
       <c r="K25" s="3" t="s">
@@ -3303,10 +3342,10 @@
         <v>30</v>
       </c>
       <c r="M25" s="14"/>
-      <c r="N25" s="96" t="s">
+      <c r="N25" s="103" t="s">
         <v>330</v>
       </c>
-      <c r="O25" s="96">
+      <c r="O25" s="103">
         <v>1</v>
       </c>
       <c r="P25" s="3" t="s">
@@ -3315,7 +3354,7 @@
       <c r="Q25" s="33">
         <v>14</v>
       </c>
-      <c r="R25" s="96">
+      <c r="R25" s="103">
         <v>2</v>
       </c>
       <c r="S25" s="3" t="s">
@@ -3328,21 +3367,21 @@
     </row>
     <row r="26" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="43"/>
-      <c r="B26" s="94"/>
+      <c r="B26" s="101"/>
       <c r="C26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="43"/>
-      <c r="F26" s="96"/>
-      <c r="G26" s="96"/>
+      <c r="F26" s="103"/>
+      <c r="G26" s="103"/>
       <c r="H26" s="3" t="s">
         <v>298</v>
       </c>
       <c r="I26" s="33">
         <v>18</v>
       </c>
-      <c r="J26" s="96"/>
+      <c r="J26" s="103"/>
       <c r="K26" s="3" t="s">
         <v>304</v>
       </c>
@@ -3350,22 +3389,22 @@
         <v>9</v>
       </c>
       <c r="M26" s="14"/>
-      <c r="N26" s="96"/>
-      <c r="O26" s="96"/>
+      <c r="N26" s="103"/>
+      <c r="O26" s="103"/>
       <c r="P26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="Q26" s="33">
         <v>7</v>
       </c>
-      <c r="R26" s="96"/>
+      <c r="R26" s="103"/>
       <c r="S26" s="3"/>
       <c r="T26" s="33"/>
       <c r="U26" s="14"/>
     </row>
     <row r="27" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="43"/>
-      <c r="B27" s="93">
+      <c r="B27" s="100">
         <v>0.52083333333333337</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -3375,10 +3414,10 @@
         <v>54</v>
       </c>
       <c r="E27" s="43"/>
-      <c r="F27" s="95" t="s">
+      <c r="F27" s="102" t="s">
         <v>358</v>
       </c>
-      <c r="G27" s="95">
+      <c r="G27" s="102">
         <v>3</v>
       </c>
       <c r="H27" s="9" t="s">
@@ -3387,8 +3426,8 @@
       <c r="I27" s="31">
         <v>23</v>
       </c>
-      <c r="J27" s="95">
-        <v>2</v>
+      <c r="J27" s="102">
+        <v>3</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>301</v>
@@ -3397,10 +3436,10 @@
         <v>21</v>
       </c>
       <c r="M27" s="14"/>
-      <c r="N27" s="95" t="s">
+      <c r="N27" s="102" t="s">
         <v>331</v>
       </c>
-      <c r="O27" s="95">
+      <c r="O27" s="102">
         <v>2</v>
       </c>
       <c r="P27" s="9" t="s">
@@ -3409,7 +3448,7 @@
       <c r="Q27" s="31">
         <v>20</v>
       </c>
-      <c r="R27" s="95">
+      <c r="R27" s="102">
         <v>2</v>
       </c>
       <c r="S27" s="9" t="s">
@@ -3422,7 +3461,7 @@
     </row>
     <row r="28" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="43"/>
-      <c r="B28" s="93"/>
+      <c r="B28" s="100"/>
       <c r="C28" s="9" t="s">
         <v>69</v>
       </c>
@@ -3430,15 +3469,15 @@
         <v>53</v>
       </c>
       <c r="E28" s="43"/>
-      <c r="F28" s="95"/>
-      <c r="G28" s="95"/>
+      <c r="F28" s="102"/>
+      <c r="G28" s="102"/>
       <c r="H28" s="9" t="s">
         <v>308</v>
       </c>
       <c r="I28" s="31">
         <v>28</v>
       </c>
-      <c r="J28" s="95"/>
+      <c r="J28" s="102"/>
       <c r="K28" s="9" t="s">
         <v>302</v>
       </c>
@@ -3446,22 +3485,22 @@
         <v>14</v>
       </c>
       <c r="M28" s="14"/>
-      <c r="N28" s="95"/>
-      <c r="O28" s="95"/>
+      <c r="N28" s="102"/>
+      <c r="O28" s="102"/>
       <c r="P28" s="9" t="s">
         <v>342</v>
       </c>
       <c r="Q28" s="31">
         <v>8</v>
       </c>
-      <c r="R28" s="95"/>
+      <c r="R28" s="102"/>
       <c r="S28" s="9"/>
       <c r="T28" s="31"/>
       <c r="U28" s="14"/>
     </row>
     <row r="29" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="43"/>
-      <c r="B29" s="94">
+      <c r="B29" s="101">
         <v>0.59722222222222221</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -3471,10 +3510,10 @@
         <v>28</v>
       </c>
       <c r="E29" s="43"/>
-      <c r="F29" s="96" t="s">
+      <c r="F29" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="G29" s="96">
+      <c r="G29" s="103">
         <v>1</v>
       </c>
       <c r="H29" s="3" t="s">
@@ -3483,7 +3522,7 @@
       <c r="I29" s="33">
         <v>10</v>
       </c>
-      <c r="J29" s="96">
+      <c r="J29" s="103">
         <v>3</v>
       </c>
       <c r="K29" s="3" t="s">
@@ -3493,10 +3532,10 @@
         <v>19</v>
       </c>
       <c r="M29" s="14"/>
-      <c r="N29" s="96" t="s">
+      <c r="N29" s="103" t="s">
         <v>332</v>
       </c>
-      <c r="O29" s="96">
+      <c r="O29" s="103">
         <v>3</v>
       </c>
       <c r="P29" s="3" t="s">
@@ -3505,7 +3544,7 @@
       <c r="Q29" s="33">
         <v>23</v>
       </c>
-      <c r="R29" s="96">
+      <c r="R29" s="103">
         <v>3</v>
       </c>
       <c r="S29" s="3" t="s">
@@ -3518,21 +3557,21 @@
     </row>
     <row r="30" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="43"/>
-      <c r="B30" s="94"/>
+      <c r="B30" s="101"/>
       <c r="C30" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="43"/>
-      <c r="F30" s="96"/>
-      <c r="G30" s="96"/>
+      <c r="F30" s="103"/>
+      <c r="G30" s="103"/>
       <c r="H30" s="3" t="s">
         <v>293</v>
       </c>
       <c r="I30" s="33">
         <v>14</v>
       </c>
-      <c r="J30" s="96"/>
+      <c r="J30" s="103"/>
       <c r="K30" s="3" t="s">
         <v>296</v>
       </c>
@@ -3540,15 +3579,15 @@
         <v>35</v>
       </c>
       <c r="M30" s="14"/>
-      <c r="N30" s="96"/>
-      <c r="O30" s="96"/>
+      <c r="N30" s="103"/>
+      <c r="O30" s="103"/>
       <c r="P30" s="3" t="s">
         <v>308</v>
       </c>
       <c r="Q30" s="33">
         <v>28</v>
       </c>
-      <c r="R30" s="96"/>
+      <c r="R30" s="103"/>
       <c r="S30" s="3" t="s">
         <v>304</v>
       </c>
@@ -3559,7 +3598,7 @@
     </row>
     <row r="31" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="43"/>
-      <c r="B31" s="93">
+      <c r="B31" s="100">
         <v>0.60416666666666663</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -3569,10 +3608,10 @@
         <v>30</v>
       </c>
       <c r="E31" s="43"/>
-      <c r="F31" s="95" t="s">
+      <c r="F31" s="102" t="s">
         <v>324</v>
       </c>
-      <c r="G31" s="95">
+      <c r="G31" s="102">
         <v>2</v>
       </c>
       <c r="H31" s="9" t="s">
@@ -3581,7 +3620,7 @@
       <c r="I31" s="31">
         <v>20</v>
       </c>
-      <c r="J31" s="95">
+      <c r="J31" s="102">
         <v>2</v>
       </c>
       <c r="K31" s="9" t="s">
@@ -3591,10 +3630,10 @@
         <v>15</v>
       </c>
       <c r="M31" s="14"/>
-      <c r="N31" s="95" t="s">
+      <c r="N31" s="102" t="s">
         <v>333</v>
       </c>
-      <c r="O31" s="95">
+      <c r="O31" s="102">
         <v>3</v>
       </c>
       <c r="P31" s="9" t="s">
@@ -3603,7 +3642,7 @@
       <c r="Q31" s="31">
         <v>19</v>
       </c>
-      <c r="R31" s="95">
+      <c r="R31" s="102">
         <v>2</v>
       </c>
       <c r="S31" s="9" t="s">
@@ -3616,21 +3655,21 @@
     </row>
     <row r="32" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="43"/>
-      <c r="B32" s="93"/>
+      <c r="B32" s="100"/>
       <c r="C32" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="43"/>
-      <c r="F32" s="95"/>
-      <c r="G32" s="95"/>
+      <c r="F32" s="102"/>
+      <c r="G32" s="102"/>
       <c r="H32" s="9" t="s">
         <v>342</v>
       </c>
       <c r="I32" s="31">
         <v>8</v>
       </c>
-      <c r="J32" s="95"/>
+      <c r="J32" s="102"/>
       <c r="K32" s="9" t="s">
         <v>357</v>
       </c>
@@ -3638,15 +3677,15 @@
         <v>12</v>
       </c>
       <c r="M32" s="14"/>
-      <c r="N32" s="95"/>
-      <c r="O32" s="95"/>
+      <c r="N32" s="102"/>
+      <c r="O32" s="102"/>
       <c r="P32" s="9" t="s">
         <v>296</v>
       </c>
       <c r="Q32" s="31">
         <v>35</v>
       </c>
-      <c r="R32" s="95"/>
+      <c r="R32" s="102"/>
       <c r="S32" s="9" t="s">
         <v>300</v>
       </c>
@@ -3661,10 +3700,10 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="43"/>
-      <c r="F33" s="96" t="s">
+      <c r="F33" s="103" t="s">
         <v>325</v>
       </c>
-      <c r="G33" s="96">
+      <c r="G33" s="103">
         <v>3</v>
       </c>
       <c r="H33" s="3" t="s">
@@ -3673,7 +3712,7 @@
       <c r="I33" s="33">
         <v>25</v>
       </c>
-      <c r="J33" s="96">
+      <c r="J33" s="103">
         <v>3</v>
       </c>
       <c r="K33" s="3" t="s">
@@ -3683,10 +3722,10 @@
         <v>36</v>
       </c>
       <c r="M33" s="14"/>
-      <c r="N33" s="96" t="s">
+      <c r="N33" s="103" t="s">
         <v>334</v>
       </c>
-      <c r="O33" s="96">
+      <c r="O33" s="103">
         <v>3</v>
       </c>
       <c r="P33" s="3" t="s">
@@ -3695,7 +3734,7 @@
       <c r="Q33" s="33">
         <v>21</v>
       </c>
-      <c r="R33" s="96">
+      <c r="R33" s="103">
         <v>3</v>
       </c>
       <c r="S33" s="3" t="s">
@@ -3712,27 +3751,27 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="43"/>
-      <c r="F34" s="96"/>
-      <c r="G34" s="96"/>
+      <c r="F34" s="103"/>
+      <c r="G34" s="103"/>
       <c r="H34" s="3" t="s">
         <v>312</v>
       </c>
       <c r="I34" s="33">
         <v>43</v>
       </c>
-      <c r="J34" s="96"/>
+      <c r="J34" s="103"/>
       <c r="K34" s="3"/>
       <c r="L34" s="33"/>
       <c r="M34" s="14"/>
-      <c r="N34" s="96"/>
-      <c r="O34" s="96"/>
+      <c r="N34" s="103"/>
+      <c r="O34" s="103"/>
       <c r="P34" s="3" t="s">
         <v>310</v>
       </c>
       <c r="Q34" s="33">
         <v>31</v>
       </c>
-      <c r="R34" s="96"/>
+      <c r="R34" s="103"/>
       <c r="S34" s="3" t="s">
         <v>288</v>
       </c>
@@ -3747,10 +3786,10 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="11"/>
-      <c r="F35" s="95" t="s">
+      <c r="F35" s="102" t="s">
         <v>326</v>
       </c>
-      <c r="G35" s="95">
+      <c r="G35" s="102">
         <v>3</v>
       </c>
       <c r="H35" s="9" t="s">
@@ -3759,7 +3798,7 @@
       <c r="I35" s="31">
         <v>10</v>
       </c>
-      <c r="J35" s="95">
+      <c r="J35" s="102">
         <v>3</v>
       </c>
       <c r="K35" s="9" t="s">
@@ -3769,10 +3808,10 @@
         <v>40</v>
       </c>
       <c r="M35" s="14"/>
-      <c r="N35" s="95" t="s">
+      <c r="N35" s="102" t="s">
         <v>335</v>
       </c>
-      <c r="O35" s="95">
+      <c r="O35" s="102">
         <v>3</v>
       </c>
       <c r="P35" s="9" t="s">
@@ -3781,7 +3820,7 @@
       <c r="Q35" s="31">
         <v>25</v>
       </c>
-      <c r="R35" s="95">
+      <c r="R35" s="102">
         <v>3</v>
       </c>
       <c r="S35" s="9" t="s">
@@ -3798,27 +3837,27 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="11"/>
-      <c r="F36" s="95"/>
-      <c r="G36" s="95"/>
+      <c r="F36" s="102"/>
+      <c r="G36" s="102"/>
       <c r="H36" s="9" t="s">
         <v>274</v>
       </c>
       <c r="I36" s="31">
         <v>28</v>
       </c>
-      <c r="J36" s="95"/>
+      <c r="J36" s="102"/>
       <c r="K36" s="9"/>
       <c r="L36" s="31"/>
       <c r="M36" s="14"/>
-      <c r="N36" s="95"/>
-      <c r="O36" s="95"/>
+      <c r="N36" s="102"/>
+      <c r="O36" s="102"/>
       <c r="P36" s="9" t="s">
         <v>312</v>
       </c>
       <c r="Q36" s="31">
         <v>43</v>
       </c>
-      <c r="R36" s="95"/>
+      <c r="R36" s="102"/>
       <c r="S36" s="9" t="s">
         <v>134</v>
       </c>
@@ -6060,6 +6099,7 @@
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="N13:N14"/>
+    <mergeCell ref="J13:J14"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="F5:F6"/>
@@ -6071,6 +6111,10 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="N7:N8"/>
     <mergeCell ref="O7:O8"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
     <mergeCell ref="N19:N20"/>
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="N25:N26"/>
@@ -6088,6 +6132,9 @@
     <mergeCell ref="G25:G26"/>
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="N15:N16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J19:J20"/>
     <mergeCell ref="F35:F36"/>
     <mergeCell ref="N35:N36"/>
     <mergeCell ref="G27:G28"/>
@@ -6117,20 +6164,12 @@
     <mergeCell ref="O21:O22"/>
     <mergeCell ref="O27:O28"/>
     <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J19:J20"/>
     <mergeCell ref="J21:J22"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="R35:R36"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="R5:R6"/>
@@ -6157,9 +6196,9 @@
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="G23:G24"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="F19:F20"/>
@@ -6172,9 +6211,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6190,10 +6231,14 @@
     <col min="10" max="10" width="9.85546875" style="35" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="8.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" style="35" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="35"/>
+    <col min="14" max="14" width="16" style="94" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="94" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="35"/>
+    <col min="17" max="20" width="10.28515625" style="35" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>13</v>
       </c>
@@ -6233,8 +6278,29 @@
       <c r="M1" s="30" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="O1" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>408</v>
+      </c>
+      <c r="Q1" s="30" t="s">
+        <v>409</v>
+      </c>
+      <c r="R1" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="S1" s="30" t="s">
+        <v>411</v>
+      </c>
+      <c r="T1" s="30" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="41">
         <v>1</v>
       </c>
@@ -6271,14 +6337,37 @@
       <c r="K2" s="45">
         <v>1</v>
       </c>
-      <c r="L2" s="97" t="s">
+      <c r="L2" s="108" t="s">
         <v>362</v>
       </c>
-      <c r="M2" s="98" t="s">
+      <c r="M2" s="109" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="95" t="str">
+        <f>CONCATENATE(B2," ", C2)</f>
+        <v>Jake Jorde</v>
+      </c>
+      <c r="O2" s="95" t="str">
+        <f>CONCATENATE(F2," ", G2)</f>
+        <v>Jeff Herberger</v>
+      </c>
+      <c r="P2" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="45">
+        <v>3</v>
+      </c>
+      <c r="R2" s="45">
+        <v>3</v>
+      </c>
+      <c r="S2" s="45">
+        <v>2</v>
+      </c>
+      <c r="T2" s="45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="41">
         <v>1</v>
       </c>
@@ -6315,10 +6404,33 @@
       <c r="K3" s="45">
         <v>1</v>
       </c>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L3" s="108"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="95" t="str">
+        <f t="shared" ref="N3:N9" si="3">CONCATENATE(B3," ", C3)</f>
+        <v>Jim Clark</v>
+      </c>
+      <c r="O3" s="95" t="str">
+        <f t="shared" ref="O3:O10" si="4">CONCATENATE(F3," ", G3)</f>
+        <v>Mike Levitt</v>
+      </c>
+      <c r="P3" s="46">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="46">
+        <v>2</v>
+      </c>
+      <c r="R3" s="46">
+        <v>2</v>
+      </c>
+      <c r="S3" s="46">
+        <v>2</v>
+      </c>
+      <c r="T3" s="46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="41">
         <v>1</v>
       </c>
@@ -6355,10 +6467,33 @@
       <c r="K4" s="45">
         <v>1</v>
       </c>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L4" s="108"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="95" t="str">
+        <f t="shared" si="3"/>
+        <v>Aaron Wald</v>
+      </c>
+      <c r="O4" s="95" t="str">
+        <f t="shared" si="4"/>
+        <v>Jon Hanson</v>
+      </c>
+      <c r="P4" s="47">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="47">
+        <v>2</v>
+      </c>
+      <c r="R4" s="47">
+        <v>2</v>
+      </c>
+      <c r="S4" s="47">
+        <v>2</v>
+      </c>
+      <c r="T4" s="47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="41">
         <v>1</v>
       </c>
@@ -6395,10 +6530,33 @@
       <c r="K5" s="45">
         <v>1</v>
       </c>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L5" s="108"/>
+      <c r="M5" s="109"/>
+      <c r="N5" s="95" t="str">
+        <f t="shared" si="3"/>
+        <v>Chris Callahan</v>
+      </c>
+      <c r="O5" s="95" t="str">
+        <f t="shared" si="4"/>
+        <v>Craig McDowell</v>
+      </c>
+      <c r="P5" s="48">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="48">
+        <v>1</v>
+      </c>
+      <c r="R5" s="48">
+        <v>1</v>
+      </c>
+      <c r="S5" s="48">
+        <v>1</v>
+      </c>
+      <c r="T5" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="41">
         <v>1</v>
       </c>
@@ -6435,10 +6593,35 @@
       <c r="K6" s="45">
         <v>1</v>
       </c>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L6" s="108"/>
+      <c r="M6" s="109"/>
+      <c r="N6" s="95" t="str">
+        <f t="shared" si="3"/>
+        <v>Todd Bodine</v>
+      </c>
+      <c r="O6" s="95" t="str">
+        <f t="shared" si="4"/>
+        <v>Chad Bodine</v>
+      </c>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36">
+        <f>SUM(Q2:Q5)</f>
+        <v>8</v>
+      </c>
+      <c r="R6" s="36">
+        <f>SUM(R2:R5)</f>
+        <v>8</v>
+      </c>
+      <c r="S6" s="36">
+        <f>SUM(S2:S5)</f>
+        <v>7</v>
+      </c>
+      <c r="T6" s="36">
+        <f>SUM(T2:T5)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="41">
         <v>1</v>
       </c>
@@ -6475,10 +6658,18 @@
       <c r="K7" s="45">
         <v>1</v>
       </c>
-      <c r="L7" s="98"/>
-      <c r="M7" s="98"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L7" s="108"/>
+      <c r="M7" s="109"/>
+      <c r="N7" s="95" t="str">
+        <f t="shared" si="3"/>
+        <v>Doug Wald</v>
+      </c>
+      <c r="O7" s="95" t="str">
+        <f t="shared" si="4"/>
+        <v>Brian Giesinger</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="41">
         <v>1</v>
       </c>
@@ -6515,10 +6706,18 @@
       <c r="K8" s="45">
         <v>1</v>
       </c>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L8" s="108"/>
+      <c r="M8" s="109"/>
+      <c r="N8" s="95" t="str">
+        <f t="shared" si="3"/>
+        <v>Andy Ness</v>
+      </c>
+      <c r="O8" s="95" t="str">
+        <f t="shared" si="4"/>
+        <v>David McCrory</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="41">
         <v>1</v>
       </c>
@@ -6555,10 +6754,18 @@
       <c r="K9" s="45">
         <v>1</v>
       </c>
-      <c r="L9" s="98"/>
-      <c r="M9" s="98"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L9" s="108"/>
+      <c r="M9" s="109"/>
+      <c r="N9" s="95" t="str">
+        <f t="shared" si="3"/>
+        <v>Steve Wald</v>
+      </c>
+      <c r="O9" s="95" t="str">
+        <f t="shared" si="4"/>
+        <v>Paul Plemel</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="41">
         <v>1</v>
       </c>
@@ -6592,13 +6799,25 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="K10" s="45">
-        <v>1</v>
-      </c>
-      <c r="L10" s="98"/>
-      <c r="M10" s="98"/>
-    </row>
-    <row r="11" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K10" s="46">
+        <v>2</v>
+      </c>
+      <c r="L10" s="106" t="s">
+        <v>363</v>
+      </c>
+      <c r="M10" s="107" t="s">
+        <v>195</v>
+      </c>
+      <c r="N10" s="96" t="str">
+        <f>CONCATENATE(B10," ", C10)</f>
+        <v>Scott Hinners</v>
+      </c>
+      <c r="O10" s="96" t="str">
+        <f t="shared" si="4"/>
+        <v>Rick Levitt</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="41">
         <v>1</v>
       </c>
@@ -6635,14 +6854,18 @@
       <c r="K11" s="46">
         <v>2</v>
       </c>
-      <c r="L11" s="99" t="s">
-        <v>363</v>
-      </c>
-      <c r="M11" s="100" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L11" s="106"/>
+      <c r="M11" s="107"/>
+      <c r="N11" s="96" t="str">
+        <f t="shared" ref="N11:N13" si="5">CONCATENATE(B11," ", C11)</f>
+        <v>Jeff Wald</v>
+      </c>
+      <c r="O11" s="96" t="str">
+        <f t="shared" ref="O11:O13" si="6">CONCATENATE(F11," ", G11)</f>
+        <v>Mike Schuette</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="41">
         <v>1</v>
       </c>
@@ -6679,10 +6902,18 @@
       <c r="K12" s="46">
         <v>2</v>
       </c>
-      <c r="L12" s="99"/>
-      <c r="M12" s="100"/>
-    </row>
-    <row r="13" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L12" s="106"/>
+      <c r="M12" s="107"/>
+      <c r="N12" s="96" t="str">
+        <f t="shared" si="5"/>
+        <v>Wayne Podolak</v>
+      </c>
+      <c r="O12" s="96" t="str">
+        <f t="shared" si="6"/>
+        <v>John Blackburn</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="39">
         <v>2</v>
       </c>
@@ -6719,10 +6950,18 @@
       <c r="K13" s="46">
         <v>2</v>
       </c>
-      <c r="L13" s="99"/>
-      <c r="M13" s="100"/>
-    </row>
-    <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L13" s="106"/>
+      <c r="M13" s="107"/>
+      <c r="N13" s="96" t="str">
+        <f t="shared" si="5"/>
+        <v>Bob Holso</v>
+      </c>
+      <c r="O13" s="96" t="str">
+        <f t="shared" si="6"/>
+        <v>Dennis Wurmlinger</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="39">
         <v>2</v>
       </c>
@@ -6756,13 +6995,13 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="K14" s="46">
-        <v>2</v>
-      </c>
-      <c r="L14" s="99"/>
-      <c r="M14" s="100"/>
-    </row>
-    <row r="15" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K14" s="93"/>
+      <c r="L14" s="106"/>
+      <c r="M14" s="107"/>
+      <c r="N14" s="97"/>
+      <c r="O14" s="97"/>
+    </row>
+    <row r="15" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="39">
         <v>2</v>
       </c>
@@ -6799,10 +7038,18 @@
       <c r="K15" s="46">
         <v>2</v>
       </c>
-      <c r="L15" s="99"/>
-      <c r="M15" s="100"/>
-    </row>
-    <row r="16" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L15" s="106"/>
+      <c r="M15" s="107"/>
+      <c r="N15" s="96" t="str">
+        <f t="shared" ref="N15" si="7">CONCATENATE(B15," ", C15)</f>
+        <v>Myron Irwin</v>
+      </c>
+      <c r="O15" s="96" t="str">
+        <f t="shared" ref="O15" si="8">CONCATENATE(F15," ", G15)</f>
+        <v>Curt Erie</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="39">
         <v>2</v>
       </c>
@@ -6836,13 +7083,13 @@
         <f>I16+E16</f>
         <v>28</v>
       </c>
-      <c r="K16" s="46">
-        <v>2</v>
-      </c>
-      <c r="L16" s="99"/>
-      <c r="M16" s="100"/>
-    </row>
-    <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K16" s="93"/>
+      <c r="L16" s="106"/>
+      <c r="M16" s="107"/>
+      <c r="N16" s="97"/>
+      <c r="O16" s="97"/>
+    </row>
+    <row r="17" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="39">
         <v>2</v>
       </c>
@@ -6876,13 +7123,13 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="K17" s="46">
-        <v>2</v>
-      </c>
-      <c r="L17" s="99"/>
-      <c r="M17" s="100"/>
-    </row>
-    <row r="18" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K17" s="93"/>
+      <c r="L17" s="106"/>
+      <c r="M17" s="107"/>
+      <c r="N17" s="97"/>
+      <c r="O17" s="97"/>
+    </row>
+    <row r="18" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="39">
         <v>2</v>
       </c>
@@ -6919,10 +7166,18 @@
       <c r="K18" s="46">
         <v>2</v>
       </c>
-      <c r="L18" s="99"/>
-      <c r="M18" s="100"/>
-    </row>
-    <row r="19" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L18" s="106"/>
+      <c r="M18" s="107"/>
+      <c r="N18" s="96" t="str">
+        <f t="shared" ref="N18:N21" si="9">CONCATENATE(B18," ", C18)</f>
+        <v>Mike Stork</v>
+      </c>
+      <c r="O18" s="96" t="str">
+        <f t="shared" ref="O18:O21" si="10">CONCATENATE(F18," ", G18)</f>
+        <v>Rick Becker</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="39">
         <v>2</v>
       </c>
@@ -6956,17 +7211,21 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="K19" s="47">
-        <v>3</v>
-      </c>
-      <c r="L19" s="101" t="s">
-        <v>364</v>
-      </c>
-      <c r="M19" s="101" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K19" s="46">
+        <v>2</v>
+      </c>
+      <c r="L19" s="106"/>
+      <c r="M19" s="107"/>
+      <c r="N19" s="96" t="str">
+        <f t="shared" si="9"/>
+        <v>Steve Francis</v>
+      </c>
+      <c r="O19" s="96" t="str">
+        <f t="shared" si="10"/>
+        <v>John Francis</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="39">
         <v>2</v>
       </c>
@@ -7000,13 +7259,21 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="K20" s="47">
-        <v>3</v>
-      </c>
-      <c r="L20" s="102"/>
-      <c r="M20" s="102"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K20" s="46">
+        <v>2</v>
+      </c>
+      <c r="L20" s="106"/>
+      <c r="M20" s="107"/>
+      <c r="N20" s="96" t="str">
+        <f t="shared" si="9"/>
+        <v>Joe Bichler</v>
+      </c>
+      <c r="O20" s="96" t="str">
+        <f t="shared" si="10"/>
+        <v>Mike Bichler</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="39">
         <v>2</v>
       </c>
@@ -7043,10 +7310,22 @@
       <c r="K21" s="47">
         <v>3</v>
       </c>
-      <c r="L21" s="102"/>
-      <c r="M21" s="102"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L21" s="104" t="s">
+        <v>364</v>
+      </c>
+      <c r="M21" s="104" t="s">
+        <v>224</v>
+      </c>
+      <c r="N21" s="98" t="str">
+        <f t="shared" si="9"/>
+        <v>Scott Hanson</v>
+      </c>
+      <c r="O21" s="98" t="str">
+        <f t="shared" si="10"/>
+        <v>Ian Quarders</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="39">
         <v>2</v>
       </c>
@@ -7083,38 +7362,46 @@
       <c r="K22" s="47">
         <v>3</v>
       </c>
-      <c r="L22" s="102"/>
-      <c r="M22" s="102"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="98" t="str">
+        <f t="shared" ref="N22:N23" si="11">CONCATENATE(B22," ", C22)</f>
+        <v>Jon Gies</v>
+      </c>
+      <c r="O22" s="98" t="str">
+        <f t="shared" ref="O22:O23" si="12">CONCATENATE(F22," ", G22)</f>
+        <v>Clyde Gies</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D23" s="39">
-        <v>21.2</v>
+        <v>21.5</v>
       </c>
       <c r="E23" s="39">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F23" s="40" t="s">
-        <v>217</v>
+        <v>160</v>
       </c>
       <c r="G23" s="40" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="H23" s="39">
-        <v>13.6</v>
+        <v>13</v>
       </c>
       <c r="I23" s="39">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J23" s="39">
         <f t="shared" si="2"/>
@@ -7123,50 +7410,66 @@
       <c r="K23" s="47">
         <v>3</v>
       </c>
-      <c r="L23" s="102"/>
-      <c r="M23" s="102"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L23" s="104"/>
+      <c r="M23" s="104"/>
+      <c r="N23" s="98" t="str">
+        <f t="shared" si="11"/>
+        <v>KT Thayer</v>
+      </c>
+      <c r="O23" s="98" t="str">
+        <f t="shared" si="12"/>
+        <v>Jeff Wurmlinger</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="37">
         <v>3</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D24" s="37">
-        <v>21.5</v>
+        <v>21.2</v>
       </c>
       <c r="E24" s="37">
-        <f t="shared" si="0"/>
-        <v>22</v>
+        <f>ROUND(D24,0)</f>
+        <v>21</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>160</v>
+        <v>217</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="H24" s="37">
-        <v>13.9</v>
+        <v>13.6</v>
       </c>
       <c r="I24" s="37">
-        <f t="shared" si="1"/>
+        <f>ROUND(H24,0)</f>
         <v>14</v>
       </c>
       <c r="J24" s="37">
-        <f t="shared" si="2"/>
-        <v>36</v>
+        <f>I24+E24</f>
+        <v>35</v>
       </c>
       <c r="K24" s="47">
         <v>3</v>
       </c>
-      <c r="L24" s="102"/>
-      <c r="M24" s="102"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L24" s="104"/>
+      <c r="M24" s="104"/>
+      <c r="N24" s="98" t="str">
+        <f t="shared" ref="N24:N27" si="13">CONCATENATE(B24," ", C24)</f>
+        <v>Joel Van Dyk</v>
+      </c>
+      <c r="O24" s="98" t="str">
+        <f t="shared" ref="O24:O27" si="14">CONCATENATE(F24," ", G24)</f>
+        <v>Shawn Dumphy</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="37">
         <v>3</v>
       </c>
@@ -7203,10 +7506,18 @@
       <c r="K25" s="47">
         <v>3</v>
       </c>
-      <c r="L25" s="102"/>
-      <c r="M25" s="102"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L25" s="104"/>
+      <c r="M25" s="104"/>
+      <c r="N25" s="98" t="str">
+        <f t="shared" si="13"/>
+        <v>Dewey Wald</v>
+      </c>
+      <c r="O25" s="98" t="str">
+        <f t="shared" si="14"/>
+        <v>Patti Wald</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="37">
         <v>3</v>
       </c>
@@ -7243,10 +7554,18 @@
       <c r="K26" s="47">
         <v>3</v>
       </c>
-      <c r="L26" s="102"/>
-      <c r="M26" s="102"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L26" s="104"/>
+      <c r="M26" s="104"/>
+      <c r="N26" s="98" t="str">
+        <f t="shared" si="13"/>
+        <v>Derek Gulbransen</v>
+      </c>
+      <c r="O26" s="98" t="str">
+        <f t="shared" si="14"/>
+        <v>Joel Pullis</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="37">
         <v>3</v>
       </c>
@@ -7280,17 +7599,21 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="K27" s="48">
-        <v>4</v>
-      </c>
-      <c r="L27" s="103" t="s">
-        <v>365</v>
-      </c>
-      <c r="M27" s="103" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K27" s="47">
+        <v>3</v>
+      </c>
+      <c r="L27" s="104"/>
+      <c r="M27" s="104"/>
+      <c r="N27" s="98" t="str">
+        <f t="shared" si="13"/>
+        <v>Brad Epker</v>
+      </c>
+      <c r="O27" s="98" t="str">
+        <f t="shared" si="14"/>
+        <v>Jeremy Gies</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="37">
         <v>3</v>
       </c>
@@ -7327,10 +7650,22 @@
       <c r="K28" s="48">
         <v>4</v>
       </c>
-      <c r="L28" s="104"/>
-      <c r="M28" s="104"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L28" s="105" t="s">
+        <v>365</v>
+      </c>
+      <c r="M28" s="105" t="s">
+        <v>234</v>
+      </c>
+      <c r="N28" s="99" t="str">
+        <f t="shared" ref="N28" si="15">CONCATENATE(B28," ", C28)</f>
+        <v>Darryl Podolak</v>
+      </c>
+      <c r="O28" s="99" t="str">
+        <f t="shared" ref="O28" si="16">CONCATENATE(F28," ", G28)</f>
+        <v>Dick Dadisman</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="37">
         <v>3</v>
       </c>
@@ -7367,10 +7702,18 @@
       <c r="K29" s="48">
         <v>4</v>
       </c>
-      <c r="L29" s="104"/>
-      <c r="M29" s="104"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L29" s="105"/>
+      <c r="M29" s="105"/>
+      <c r="N29" s="99" t="str">
+        <f t="shared" ref="N29:N31" si="17">CONCATENATE(B29," ", C29)</f>
+        <v>Dwane Liuska</v>
+      </c>
+      <c r="O29" s="99" t="str">
+        <f t="shared" ref="O29:O31" si="18">CONCATENATE(F29," ", G29)</f>
+        <v>Marshal Hagen</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="37">
         <v>3</v>
       </c>
@@ -7407,10 +7750,18 @@
       <c r="K30" s="48">
         <v>4</v>
       </c>
-      <c r="L30" s="104"/>
-      <c r="M30" s="104"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L30" s="105"/>
+      <c r="M30" s="105"/>
+      <c r="N30" s="99" t="str">
+        <f t="shared" si="17"/>
+        <v>Bob Cruzan</v>
+      </c>
+      <c r="O30" s="99" t="str">
+        <f t="shared" si="18"/>
+        <v>Justin Kosanovich</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="37">
         <v>3</v>
       </c>
@@ -7447,10 +7798,18 @@
       <c r="K31" s="48">
         <v>4</v>
       </c>
-      <c r="L31" s="104"/>
-      <c r="M31" s="104"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L31" s="105"/>
+      <c r="M31" s="105"/>
+      <c r="N31" s="99" t="str">
+        <f t="shared" si="17"/>
+        <v>Garth Billsten</v>
+      </c>
+      <c r="O31" s="99" t="str">
+        <f t="shared" si="18"/>
+        <v>Christopher Stafford</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="37">
         <v>3</v>
       </c>
@@ -7487,10 +7846,18 @@
       <c r="K32" s="48">
         <v>4</v>
       </c>
-      <c r="L32" s="104"/>
-      <c r="M32" s="104"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L32" s="105"/>
+      <c r="M32" s="105"/>
+      <c r="N32" s="99" t="str">
+        <f t="shared" ref="N32:N34" si="19">CONCATENATE(B32," ", C32)</f>
+        <v>Andy Podolak</v>
+      </c>
+      <c r="O32" s="99" t="str">
+        <f t="shared" ref="O32:O34" si="20">CONCATENATE(F32," ", G32)</f>
+        <v>Mitch Mondala</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="37">
         <v>3</v>
       </c>
@@ -7527,10 +7894,18 @@
       <c r="K33" s="48">
         <v>4</v>
       </c>
-      <c r="L33" s="104"/>
-      <c r="M33" s="104"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L33" s="105"/>
+      <c r="M33" s="105"/>
+      <c r="N33" s="99" t="str">
+        <f t="shared" si="19"/>
+        <v>Guy Rasmussen</v>
+      </c>
+      <c r="O33" s="99" t="str">
+        <f t="shared" si="20"/>
+        <v>Jeanne Rasmussen</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="37">
         <v>3</v>
       </c>
@@ -7567,16 +7942,24 @@
       <c r="K34" s="48">
         <v>4</v>
       </c>
-      <c r="L34" s="104"/>
-      <c r="M34" s="104"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L34" s="105"/>
+      <c r="M34" s="105"/>
+      <c r="N34" s="99" t="str">
+        <f t="shared" si="19"/>
+        <v>Laura Roseleip</v>
+      </c>
+      <c r="O34" s="99" t="str">
+        <f t="shared" si="20"/>
+        <v>Mike Roseleip</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="K39" s="49"/>
     </row>
-    <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="15.75" x14ac:dyDescent="0.2">
       <c r="K41" s="50"/>
     </row>
-    <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K43" s="51"/>
     </row>
   </sheetData>
@@ -7584,14 +7967,14 @@
     <sortCondition ref="J2:J34"/>
   </sortState>
   <mergeCells count="8">
-    <mergeCell ref="L2:L10"/>
-    <mergeCell ref="L11:L18"/>
-    <mergeCell ref="L19:L26"/>
-    <mergeCell ref="L27:L34"/>
-    <mergeCell ref="M2:M10"/>
-    <mergeCell ref="M11:M18"/>
-    <mergeCell ref="M19:M26"/>
-    <mergeCell ref="M27:M34"/>
+    <mergeCell ref="L2:L9"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="L21:L27"/>
+    <mergeCell ref="M21:M27"/>
+    <mergeCell ref="L28:L34"/>
+    <mergeCell ref="M28:M34"/>
+    <mergeCell ref="L10:L20"/>
+    <mergeCell ref="M10:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixes during monster 2013
</commit_message>
<xml_diff>
--- a/monster2013/Monster All.xlsx
+++ b/monster2013/Monster All.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="15240" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="15240" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Monster" sheetId="6" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Purse" sheetId="11" r:id="rId3"/>
     <sheet name="Field" sheetId="7" r:id="rId4"/>
     <sheet name="Course" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="456">
   <si>
     <t>Total</t>
   </si>
@@ -1257,6 +1258,135 @@
   </si>
   <si>
     <t>HR Flight 4</t>
+  </si>
+  <si>
+    <t>Round 1</t>
+  </si>
+  <si>
+    <t>Round 2</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Hcp</t>
+  </si>
+  <si>
+    <t>Net</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Callahan - McDowell</t>
+  </si>
+  <si>
+    <t>Plemel - Wald</t>
+  </si>
+  <si>
+    <t>Hinners - Levitt</t>
+  </si>
+  <si>
+    <t>Giesinger - Wald</t>
+  </si>
+  <si>
+    <t>Schuette - Wald</t>
+  </si>
+  <si>
+    <t>Hanson - Wald</t>
+  </si>
+  <si>
+    <t>Blackburn - Podolak</t>
+  </si>
+  <si>
+    <t>Herberger - Jorde</t>
+  </si>
+  <si>
+    <t>McCrory - Ness</t>
+  </si>
+  <si>
+    <t>Bodine - Bodine</t>
+  </si>
+  <si>
+    <t>Clark - Levitt</t>
+  </si>
+  <si>
+    <t>Jim Clark</t>
+  </si>
+  <si>
+    <t>Thayer - Wurmlinger</t>
+  </si>
+  <si>
+    <t>Francis - Francis</t>
+  </si>
+  <si>
+    <t>Hanson - Quarders</t>
+  </si>
+  <si>
+    <t>Haseleu - Hefta</t>
+  </si>
+  <si>
+    <t>Erie - Irwin</t>
+  </si>
+  <si>
+    <t>Gies - Gies</t>
+  </si>
+  <si>
+    <t>Becker - Stork</t>
+  </si>
+  <si>
+    <t>Haug - Walker</t>
+  </si>
+  <si>
+    <t>Evenson - Redfern</t>
+  </si>
+  <si>
+    <t>Holso - Wurmlinger</t>
+  </si>
+  <si>
+    <t>Bichler - Bichler</t>
+  </si>
+  <si>
+    <t>Epker - Gies</t>
+  </si>
+  <si>
+    <t>Hagen - Liuska</t>
+  </si>
+  <si>
+    <t>Cruzan - Kosanovich</t>
+  </si>
+  <si>
+    <t>Dumphy - Van Dyk</t>
+  </si>
+  <si>
+    <t>Mondala - Podolak</t>
+  </si>
+  <si>
+    <t>Roseleip - Roseleip</t>
+  </si>
+  <si>
+    <t>Dadisman - Podolak</t>
+  </si>
+  <si>
+    <t>Rasmussen - Rasmussen</t>
+  </si>
+  <si>
+    <t>Wald - Wald</t>
+  </si>
+  <si>
+    <t>Gulbransen - Pullis</t>
+  </si>
+  <si>
+    <t>Billsten - Stafford</t>
   </si>
 </sst>
 </file>
@@ -1268,7 +1398,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0_);\(0\)"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1368,8 +1498,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1471,8 +1607,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5DEB3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADD8E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAFAD2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1510,6 +1664,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1519,7 +1688,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1743,19 +1912,25 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="18" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="18" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1769,11 +1944,32 @@
     <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2206,7 +2402,7 @@
     </row>
     <row r="3" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="43"/>
-      <c r="B3" s="100">
+      <c r="B3" s="102">
         <v>0.40277777777777773</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -2216,10 +2412,10 @@
         <v>286</v>
       </c>
       <c r="E3" s="43"/>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="101" t="s">
         <v>315</v>
       </c>
-      <c r="G3" s="102">
+      <c r="G3" s="101">
         <v>1</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -2228,7 +2424,7 @@
       <c r="I3" s="31">
         <v>8</v>
       </c>
-      <c r="J3" s="102">
+      <c r="J3" s="101">
         <v>1</v>
       </c>
       <c r="K3" s="9" t="s">
@@ -2238,10 +2434,10 @@
         <v>16</v>
       </c>
       <c r="M3" s="10"/>
-      <c r="N3" s="102" t="s">
+      <c r="N3" s="101" t="s">
         <v>369</v>
       </c>
-      <c r="O3" s="102">
+      <c r="O3" s="101">
         <v>1</v>
       </c>
       <c r="P3" s="9" t="s">
@@ -2250,7 +2446,7 @@
       <c r="Q3" s="31">
         <v>8</v>
       </c>
-      <c r="R3" s="102">
+      <c r="R3" s="101">
         <v>1</v>
       </c>
       <c r="S3" s="9" t="s">
@@ -2263,7 +2459,7 @@
     </row>
     <row r="4" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="43"/>
-      <c r="B4" s="100"/>
+      <c r="B4" s="102"/>
       <c r="C4" s="9" t="s">
         <v>60</v>
       </c>
@@ -2271,15 +2467,15 @@
         <v>62</v>
       </c>
       <c r="E4" s="43"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
       <c r="H4" s="12" t="s">
         <v>256</v>
       </c>
       <c r="I4" s="34">
         <v>2</v>
       </c>
-      <c r="J4" s="102"/>
+      <c r="J4" s="101"/>
       <c r="K4" s="13" t="s">
         <v>260</v>
       </c>
@@ -2287,15 +2483,15 @@
         <v>7</v>
       </c>
       <c r="M4" s="14"/>
-      <c r="N4" s="102"/>
-      <c r="O4" s="102"/>
+      <c r="N4" s="101"/>
+      <c r="O4" s="101"/>
       <c r="P4" s="12" t="s">
         <v>256</v>
       </c>
       <c r="Q4" s="34">
         <v>2</v>
       </c>
-      <c r="R4" s="102"/>
+      <c r="R4" s="101"/>
       <c r="S4" s="13" t="s">
         <v>258</v>
       </c>
@@ -2306,7 +2502,7 @@
     </row>
     <row r="5" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="43"/>
-      <c r="B5" s="101">
+      <c r="B5" s="103">
         <v>0.40972222222222227</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -2316,10 +2512,10 @@
         <v>57</v>
       </c>
       <c r="E5" s="43"/>
-      <c r="F5" s="103" t="s">
+      <c r="F5" s="100" t="s">
         <v>316</v>
       </c>
-      <c r="G5" s="103">
+      <c r="G5" s="100">
         <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -2328,7 +2524,7 @@
       <c r="I5" s="33">
         <v>5</v>
       </c>
-      <c r="J5" s="103">
+      <c r="J5" s="100">
         <v>1</v>
       </c>
       <c r="K5" s="3" t="s">
@@ -2338,10 +2534,10 @@
         <v>2</v>
       </c>
       <c r="M5" s="14"/>
-      <c r="N5" s="103" t="s">
+      <c r="N5" s="100" t="s">
         <v>368</v>
       </c>
-      <c r="O5" s="103">
+      <c r="O5" s="100">
         <v>1</v>
       </c>
       <c r="P5" s="3" t="s">
@@ -2350,7 +2546,7 @@
       <c r="Q5" s="33">
         <v>5</v>
       </c>
-      <c r="R5" s="103">
+      <c r="R5" s="100">
         <v>2</v>
       </c>
       <c r="S5" s="3" t="s">
@@ -2363,7 +2559,7 @@
     </row>
     <row r="6" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="43"/>
-      <c r="B6" s="101">
+      <c r="B6" s="103">
         <v>0.40972222222222227</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -2373,15 +2569,15 @@
         <v>58</v>
       </c>
       <c r="E6" s="43"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
       <c r="H6" s="3" t="s">
         <v>262</v>
       </c>
       <c r="I6" s="33">
         <v>12</v>
       </c>
-      <c r="J6" s="103"/>
+      <c r="J6" s="100"/>
       <c r="K6" s="3" t="s">
         <v>264</v>
       </c>
@@ -2389,15 +2585,15 @@
         <v>9</v>
       </c>
       <c r="M6" s="14"/>
-      <c r="N6" s="103"/>
-      <c r="O6" s="103"/>
+      <c r="N6" s="100"/>
+      <c r="O6" s="100"/>
       <c r="P6" s="3" t="s">
         <v>262</v>
       </c>
       <c r="Q6" s="33">
         <v>12</v>
       </c>
-      <c r="R6" s="103"/>
+      <c r="R6" s="100"/>
       <c r="S6" s="3" t="s">
         <v>270</v>
       </c>
@@ -2408,7 +2604,7 @@
     </row>
     <row r="7" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="43"/>
-      <c r="B7" s="100">
+      <c r="B7" s="102">
         <v>0.41666666666666669</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -2418,10 +2614,10 @@
         <v>33</v>
       </c>
       <c r="E7" s="43"/>
-      <c r="F7" s="102" t="s">
+      <c r="F7" s="101" t="s">
         <v>317</v>
       </c>
-      <c r="G7" s="102">
+      <c r="G7" s="101">
         <v>2</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -2430,7 +2626,7 @@
       <c r="I7" s="31">
         <v>22</v>
       </c>
-      <c r="J7" s="102">
+      <c r="J7" s="101">
         <v>1</v>
       </c>
       <c r="K7" s="9" t="s">
@@ -2440,10 +2636,10 @@
         <v>6</v>
       </c>
       <c r="M7" s="14"/>
-      <c r="N7" s="102" t="s">
+      <c r="N7" s="101" t="s">
         <v>317</v>
       </c>
-      <c r="O7" s="102">
+      <c r="O7" s="101">
         <v>1</v>
       </c>
       <c r="P7" s="9" t="s">
@@ -2452,7 +2648,7 @@
       <c r="Q7" s="31">
         <v>2</v>
       </c>
-      <c r="R7" s="102">
+      <c r="R7" s="101">
         <v>1</v>
       </c>
       <c r="S7" s="9" t="s">
@@ -2465,7 +2661,7 @@
     </row>
     <row r="8" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="43"/>
-      <c r="B8" s="100">
+      <c r="B8" s="102">
         <v>0.41666666666666669</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -2475,15 +2671,15 @@
         <v>34</v>
       </c>
       <c r="E8" s="43"/>
-      <c r="F8" s="102"/>
-      <c r="G8" s="102"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
       <c r="H8" s="9" t="s">
         <v>267</v>
       </c>
       <c r="I8" s="31">
         <v>13</v>
       </c>
-      <c r="J8" s="102"/>
+      <c r="J8" s="101"/>
       <c r="K8" s="9" t="s">
         <v>269</v>
       </c>
@@ -2491,15 +2687,15 @@
         <v>10</v>
       </c>
       <c r="M8" s="14"/>
-      <c r="N8" s="102"/>
-      <c r="O8" s="102"/>
+      <c r="N8" s="101"/>
+      <c r="O8" s="101"/>
       <c r="P8" s="9" t="s">
         <v>264</v>
       </c>
       <c r="Q8" s="31">
         <v>9</v>
       </c>
-      <c r="R8" s="102"/>
+      <c r="R8" s="101"/>
       <c r="S8" s="9" t="s">
         <v>276</v>
       </c>
@@ -2510,7 +2706,7 @@
     </row>
     <row r="9" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="43"/>
-      <c r="B9" s="101">
+      <c r="B9" s="103">
         <v>0.4236111111111111</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -2520,10 +2716,10 @@
         <v>67</v>
       </c>
       <c r="E9" s="43"/>
-      <c r="F9" s="103" t="s">
+      <c r="F9" s="100" t="s">
         <v>327</v>
       </c>
-      <c r="G9" s="103">
+      <c r="G9" s="100">
         <v>1</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -2532,7 +2728,7 @@
       <c r="I9" s="33">
         <v>2</v>
       </c>
-      <c r="J9" s="103">
+      <c r="J9" s="100">
         <v>3</v>
       </c>
       <c r="K9" s="3" t="s">
@@ -2542,10 +2738,10 @@
         <v>22</v>
       </c>
       <c r="M9" s="14"/>
-      <c r="N9" s="103" t="s">
+      <c r="N9" s="100" t="s">
         <v>327</v>
       </c>
-      <c r="O9" s="103">
+      <c r="O9" s="100">
         <v>1</v>
       </c>
       <c r="P9" s="3" t="s">
@@ -2554,7 +2750,7 @@
       <c r="Q9" s="33">
         <v>16</v>
       </c>
-      <c r="R9" s="103">
+      <c r="R9" s="100">
         <v>2</v>
       </c>
       <c r="S9" s="3" t="s">
@@ -2567,7 +2763,7 @@
     </row>
     <row r="10" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="43"/>
-      <c r="B10" s="101"/>
+      <c r="B10" s="103"/>
       <c r="C10" s="3" t="s">
         <v>96</v>
       </c>
@@ -2575,15 +2771,15 @@
         <v>68</v>
       </c>
       <c r="E10" s="43"/>
-      <c r="F10" s="103"/>
-      <c r="G10" s="103"/>
+      <c r="F10" s="100"/>
+      <c r="G10" s="100"/>
       <c r="H10" s="3" t="s">
         <v>258</v>
       </c>
       <c r="I10" s="33">
         <v>5</v>
       </c>
-      <c r="J10" s="103"/>
+      <c r="J10" s="100"/>
       <c r="K10" s="3" t="s">
         <v>272</v>
       </c>
@@ -2591,15 +2787,15 @@
         <v>24</v>
       </c>
       <c r="M10" s="14"/>
-      <c r="N10" s="103"/>
-      <c r="O10" s="103"/>
+      <c r="N10" s="100"/>
+      <c r="O10" s="100"/>
       <c r="P10" s="3" t="s">
         <v>259</v>
       </c>
       <c r="Q10" s="33">
         <v>7</v>
       </c>
-      <c r="R10" s="103"/>
+      <c r="R10" s="100"/>
       <c r="S10" s="3" t="s">
         <v>282</v>
       </c>
@@ -2610,7 +2806,7 @@
     </row>
     <row r="11" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="43"/>
-      <c r="B11" s="100">
+      <c r="B11" s="102">
         <v>0.43055555555555558</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -2620,10 +2816,10 @@
         <v>51</v>
       </c>
       <c r="E11" s="43"/>
-      <c r="F11" s="102" t="s">
+      <c r="F11" s="101" t="s">
         <v>336</v>
       </c>
-      <c r="G11" s="102">
+      <c r="G11" s="101">
         <v>1</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -2632,7 +2828,7 @@
       <c r="I11" s="31">
         <v>0</v>
       </c>
-      <c r="J11" s="102">
+      <c r="J11" s="101">
         <v>2</v>
       </c>
       <c r="K11" s="9" t="s">
@@ -2642,10 +2838,10 @@
         <v>8</v>
       </c>
       <c r="M11" s="14"/>
-      <c r="N11" s="102" t="s">
+      <c r="N11" s="101" t="s">
         <v>318</v>
       </c>
-      <c r="O11" s="102">
+      <c r="O11" s="101">
         <v>3</v>
       </c>
       <c r="P11" s="9" t="s">
@@ -2654,7 +2850,7 @@
       <c r="Q11" s="31">
         <v>22</v>
       </c>
-      <c r="R11" s="102">
+      <c r="R11" s="101">
         <v>1</v>
       </c>
       <c r="S11" s="9" t="s">
@@ -2667,7 +2863,7 @@
     </row>
     <row r="12" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="43"/>
-      <c r="B12" s="100">
+      <c r="B12" s="102">
         <v>0.4236111111111111</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -2677,15 +2873,15 @@
         <v>22</v>
       </c>
       <c r="E12" s="43"/>
-      <c r="F12" s="102"/>
-      <c r="G12" s="102"/>
+      <c r="F12" s="101"/>
+      <c r="G12" s="101"/>
       <c r="H12" s="9" t="s">
         <v>276</v>
       </c>
       <c r="I12" s="31">
         <v>3</v>
       </c>
-      <c r="J12" s="102"/>
+      <c r="J12" s="101"/>
       <c r="K12" s="9" t="s">
         <v>270</v>
       </c>
@@ -2693,15 +2889,15 @@
         <v>20</v>
       </c>
       <c r="M12" s="14"/>
-      <c r="N12" s="102"/>
-      <c r="O12" s="102"/>
+      <c r="N12" s="101"/>
+      <c r="O12" s="101"/>
       <c r="P12" s="9" t="s">
         <v>272</v>
       </c>
       <c r="Q12" s="31">
         <v>24</v>
       </c>
-      <c r="R12" s="102"/>
+      <c r="R12" s="101"/>
       <c r="S12" s="9" t="s">
         <v>269</v>
       </c>
@@ -2712,7 +2908,7 @@
     </row>
     <row r="13" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="43"/>
-      <c r="B13" s="101">
+      <c r="B13" s="103">
         <v>0.4375</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -2722,10 +2918,10 @@
         <v>44</v>
       </c>
       <c r="E13" s="43"/>
-      <c r="F13" s="103" t="s">
+      <c r="F13" s="100" t="s">
         <v>360</v>
       </c>
-      <c r="G13" s="103">
+      <c r="G13" s="100">
         <v>1</v>
       </c>
       <c r="H13" s="15" t="s">
@@ -2734,7 +2930,7 @@
       <c r="I13" s="33">
         <v>8</v>
       </c>
-      <c r="J13" s="103">
+      <c r="J13" s="100">
         <v>2</v>
       </c>
       <c r="K13" s="15" t="s">
@@ -2744,10 +2940,10 @@
         <v>13</v>
       </c>
       <c r="M13" s="14"/>
-      <c r="N13" s="103" t="s">
+      <c r="N13" s="100" t="s">
         <v>328</v>
       </c>
-      <c r="O13" s="103">
+      <c r="O13" s="100">
         <v>1</v>
       </c>
       <c r="P13" s="15" t="s">
@@ -2756,7 +2952,7 @@
       <c r="Q13" s="33">
         <v>8</v>
       </c>
-      <c r="R13" s="103">
+      <c r="R13" s="100">
         <v>3</v>
       </c>
       <c r="S13" s="15" t="s">
@@ -2769,7 +2965,7 @@
     </row>
     <row r="14" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="43"/>
-      <c r="B14" s="101">
+      <c r="B14" s="103">
         <v>0.43055555555555558</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -2777,15 +2973,15 @@
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="43"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="103"/>
+      <c r="F14" s="100"/>
+      <c r="G14" s="100"/>
       <c r="H14" s="3" t="s">
         <v>278</v>
       </c>
       <c r="I14" s="33">
         <v>12</v>
       </c>
-      <c r="J14" s="103"/>
+      <c r="J14" s="100"/>
       <c r="K14" s="3" t="s">
         <v>282</v>
       </c>
@@ -2793,15 +2989,15 @@
         <v>13</v>
       </c>
       <c r="M14" s="14"/>
-      <c r="N14" s="103"/>
-      <c r="O14" s="103"/>
+      <c r="N14" s="100"/>
+      <c r="O14" s="100"/>
       <c r="P14" s="3" t="s">
         <v>278</v>
       </c>
       <c r="Q14" s="33">
         <v>12</v>
       </c>
-      <c r="R14" s="103"/>
+      <c r="R14" s="100"/>
       <c r="S14" s="3" t="s">
         <v>274</v>
       </c>
@@ -2812,7 +3008,7 @@
     </row>
     <row r="15" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="43"/>
-      <c r="B15" s="100">
+      <c r="B15" s="102">
         <v>0.44444444444444442</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -2822,10 +3018,10 @@
         <v>340</v>
       </c>
       <c r="E15" s="43"/>
-      <c r="F15" s="102" t="s">
+      <c r="F15" s="101" t="s">
         <v>328</v>
       </c>
-      <c r="G15" s="102">
+      <c r="G15" s="101">
         <v>2</v>
       </c>
       <c r="H15" s="9" t="s">
@@ -2834,7 +3030,7 @@
       <c r="I15" s="31">
         <v>11</v>
       </c>
-      <c r="J15" s="102">
+      <c r="J15" s="101">
         <v>2</v>
       </c>
       <c r="K15" s="9" t="s">
@@ -2844,10 +3040,10 @@
         <v>15</v>
       </c>
       <c r="M15" s="14"/>
-      <c r="N15" s="102" t="s">
+      <c r="N15" s="101" t="s">
         <v>319</v>
       </c>
-      <c r="O15" s="102">
+      <c r="O15" s="101">
         <v>2</v>
       </c>
       <c r="P15" s="9" t="s">
@@ -2856,7 +3052,7 @@
       <c r="Q15" s="31">
         <v>22</v>
       </c>
-      <c r="R15" s="102">
+      <c r="R15" s="101">
         <v>2</v>
       </c>
       <c r="S15" s="9" t="s">
@@ -2869,7 +3065,7 @@
     </row>
     <row r="16" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="43"/>
-      <c r="B16" s="100"/>
+      <c r="B16" s="102"/>
       <c r="C16" s="9" t="s">
         <v>52</v>
       </c>
@@ -2877,15 +3073,15 @@
         <v>342</v>
       </c>
       <c r="E16" s="43"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="102"/>
+      <c r="F16" s="101"/>
+      <c r="G16" s="101"/>
       <c r="H16" s="9" t="s">
         <v>286</v>
       </c>
       <c r="I16" s="31">
         <v>18</v>
       </c>
-      <c r="J16" s="102"/>
+      <c r="J16" s="101"/>
       <c r="K16" s="9" t="s">
         <v>280</v>
       </c>
@@ -2893,15 +3089,15 @@
         <v>17</v>
       </c>
       <c r="M16" s="14"/>
-      <c r="N16" s="102"/>
-      <c r="O16" s="102"/>
+      <c r="N16" s="101"/>
+      <c r="O16" s="101"/>
       <c r="P16" s="9" t="s">
         <v>267</v>
       </c>
       <c r="Q16" s="31">
         <v>13</v>
       </c>
-      <c r="R16" s="102"/>
+      <c r="R16" s="101"/>
       <c r="S16" s="9" t="s">
         <v>284</v>
       </c>
@@ -2912,7 +3108,7 @@
     </row>
     <row r="17" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="43"/>
-      <c r="B17" s="101">
+      <c r="B17" s="103">
         <v>0.4513888888888889</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2922,10 +3118,10 @@
         <v>21</v>
       </c>
       <c r="E17" s="43"/>
-      <c r="F17" s="103" t="s">
+      <c r="F17" s="100" t="s">
         <v>337</v>
       </c>
-      <c r="G17" s="103">
+      <c r="G17" s="100">
         <v>3</v>
       </c>
       <c r="H17" s="3" t="s">
@@ -2934,7 +3130,7 @@
       <c r="I17" s="33">
         <v>23</v>
       </c>
-      <c r="J17" s="103">
+      <c r="J17" s="100">
         <v>2</v>
       </c>
       <c r="K17" s="3" t="s">
@@ -2944,10 +3140,10 @@
         <v>12</v>
       </c>
       <c r="M17" s="14"/>
-      <c r="N17" s="103" t="s">
+      <c r="N17" s="100" t="s">
         <v>329</v>
       </c>
-      <c r="O17" s="103">
+      <c r="O17" s="100">
         <v>2</v>
       </c>
       <c r="P17" s="3" t="s">
@@ -2956,7 +3152,7 @@
       <c r="Q17" s="33">
         <v>12</v>
       </c>
-      <c r="R17" s="103">
+      <c r="R17" s="100">
         <v>2</v>
       </c>
       <c r="S17" s="3" t="s">
@@ -2969,21 +3165,21 @@
     </row>
     <row r="18" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="43"/>
-      <c r="B18" s="101"/>
+      <c r="B18" s="103"/>
       <c r="C18" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="43"/>
-      <c r="F18" s="103"/>
-      <c r="G18" s="103"/>
+      <c r="F18" s="100"/>
+      <c r="G18" s="100"/>
       <c r="H18" s="3" t="s">
         <v>288</v>
       </c>
       <c r="I18" s="33">
         <v>19</v>
       </c>
-      <c r="J18" s="103"/>
+      <c r="J18" s="100"/>
       <c r="K18" s="3" t="s">
         <v>290</v>
       </c>
@@ -2991,15 +3187,15 @@
         <v>22</v>
       </c>
       <c r="M18" s="14"/>
-      <c r="N18" s="103"/>
-      <c r="O18" s="103"/>
+      <c r="N18" s="100"/>
+      <c r="O18" s="100"/>
       <c r="P18" s="3" t="s">
         <v>290</v>
       </c>
       <c r="Q18" s="33">
         <v>22</v>
       </c>
-      <c r="R18" s="103"/>
+      <c r="R18" s="100"/>
       <c r="S18" s="3" t="s">
         <v>280</v>
       </c>
@@ -3010,7 +3206,7 @@
     </row>
     <row r="19" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="43"/>
-      <c r="B19" s="100">
+      <c r="B19" s="102">
         <v>0.45833333333333331</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -3020,10 +3216,10 @@
         <v>56</v>
       </c>
       <c r="E19" s="43"/>
-      <c r="F19" s="102" t="s">
+      <c r="F19" s="101" t="s">
         <v>338</v>
       </c>
-      <c r="G19" s="102">
+      <c r="G19" s="101">
         <v>1</v>
       </c>
       <c r="H19" s="9" t="s">
@@ -3032,7 +3228,7 @@
       <c r="I19" s="31">
         <v>12</v>
       </c>
-      <c r="J19" s="102">
+      <c r="J19" s="101">
         <v>3</v>
       </c>
       <c r="K19" s="9" t="s">
@@ -3042,10 +3238,10 @@
         <v>21</v>
       </c>
       <c r="M19" s="16"/>
-      <c r="N19" s="102" t="s">
+      <c r="N19" s="101" t="s">
         <v>322</v>
       </c>
-      <c r="O19" s="102">
+      <c r="O19" s="101">
         <v>1</v>
       </c>
       <c r="P19" s="9" t="s">
@@ -3054,7 +3250,7 @@
       <c r="Q19" s="31">
         <v>12</v>
       </c>
-      <c r="R19" s="102">
+      <c r="R19" s="101">
         <v>2</v>
       </c>
       <c r="S19" s="9" t="s">
@@ -3067,7 +3263,7 @@
     </row>
     <row r="20" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="43"/>
-      <c r="B20" s="100"/>
+      <c r="B20" s="102"/>
       <c r="C20" s="9" t="s">
         <v>308</v>
       </c>
@@ -3075,15 +3271,15 @@
         <v>64</v>
       </c>
       <c r="E20" s="43"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="102"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="101"/>
       <c r="H20" s="9" t="s">
         <v>96</v>
       </c>
       <c r="I20" s="31">
         <v>6</v>
       </c>
-      <c r="J20" s="102"/>
+      <c r="J20" s="101"/>
       <c r="K20" s="9" t="s">
         <v>310</v>
       </c>
@@ -3091,15 +3287,15 @@
         <v>31</v>
       </c>
       <c r="M20" s="14"/>
-      <c r="N20" s="102"/>
-      <c r="O20" s="102"/>
+      <c r="N20" s="101"/>
+      <c r="O20" s="101"/>
       <c r="P20" s="9" t="s">
         <v>96</v>
       </c>
       <c r="Q20" s="31">
         <v>6</v>
       </c>
-      <c r="R20" s="102"/>
+      <c r="R20" s="101"/>
       <c r="S20" s="9" t="s">
         <v>298</v>
       </c>
@@ -3110,7 +3306,7 @@
     </row>
     <row r="21" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="43"/>
-      <c r="B21" s="101">
+      <c r="B21" s="103">
         <v>0.46527777777777773</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -3120,10 +3316,10 @@
         <v>134</v>
       </c>
       <c r="E21" s="43"/>
-      <c r="F21" s="103" t="s">
+      <c r="F21" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="G21" s="103">
+      <c r="G21" s="100">
         <v>1</v>
       </c>
       <c r="H21" s="3" t="s">
@@ -3132,7 +3328,7 @@
       <c r="I21" s="33">
         <v>14</v>
       </c>
-      <c r="J21" s="103">
+      <c r="J21" s="100">
         <v>2</v>
       </c>
       <c r="K21" s="3" t="s">
@@ -3142,10 +3338,10 @@
         <v>12</v>
       </c>
       <c r="M21" s="14"/>
-      <c r="N21" s="103" t="s">
+      <c r="N21" s="100" t="s">
         <v>323</v>
       </c>
-      <c r="O21" s="103">
+      <c r="O21" s="100">
         <v>3</v>
       </c>
       <c r="P21" s="3" t="s">
@@ -3154,7 +3350,7 @@
       <c r="Q21" s="33">
         <v>21</v>
       </c>
-      <c r="R21" s="103">
+      <c r="R21" s="100">
         <v>2</v>
       </c>
       <c r="S21" s="3" t="s">
@@ -3167,7 +3363,7 @@
     </row>
     <row r="22" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="43"/>
-      <c r="B22" s="101"/>
+      <c r="B22" s="103"/>
       <c r="C22" s="3" t="s">
         <v>40</v>
       </c>
@@ -3175,15 +3371,15 @@
         <v>135</v>
       </c>
       <c r="E22" s="43"/>
-      <c r="F22" s="103"/>
-      <c r="G22" s="103"/>
+      <c r="F22" s="100"/>
+      <c r="G22" s="100"/>
       <c r="H22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I22" s="33">
         <v>7</v>
       </c>
-      <c r="J22" s="103"/>
+      <c r="J22" s="100"/>
       <c r="K22" s="3" t="s">
         <v>284</v>
       </c>
@@ -3191,15 +3387,15 @@
         <v>13</v>
       </c>
       <c r="M22" s="14"/>
-      <c r="N22" s="103"/>
-      <c r="O22" s="103"/>
+      <c r="N22" s="100"/>
+      <c r="O22" s="100"/>
       <c r="P22" s="3" t="s">
         <v>302</v>
       </c>
       <c r="Q22" s="33">
         <v>14</v>
       </c>
-      <c r="R22" s="103"/>
+      <c r="R22" s="100"/>
       <c r="S22" s="3" t="s">
         <v>286</v>
       </c>
@@ -3210,7 +3406,7 @@
     </row>
     <row r="23" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="43"/>
-      <c r="B23" s="100">
+      <c r="B23" s="102">
         <v>0.47916666666666669</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -3220,10 +3416,10 @@
         <v>353</v>
       </c>
       <c r="E23" s="43"/>
-      <c r="F23" s="102" t="s">
+      <c r="F23" s="101" t="s">
         <v>321</v>
       </c>
-      <c r="G23" s="102">
+      <c r="G23" s="101">
         <v>2</v>
       </c>
       <c r="H23" s="9" t="s">
@@ -3232,7 +3428,7 @@
       <c r="I23" s="31">
         <v>18</v>
       </c>
-      <c r="J23" s="102">
+      <c r="J23" s="101">
         <v>3</v>
       </c>
       <c r="K23" s="9" t="s">
@@ -3242,10 +3438,10 @@
         <v>27</v>
       </c>
       <c r="M23" s="14"/>
-      <c r="N23" s="102" t="s">
+      <c r="N23" s="101" t="s">
         <v>324</v>
       </c>
-      <c r="O23" s="102">
+      <c r="O23" s="101">
         <v>1</v>
       </c>
       <c r="P23" s="9" t="s">
@@ -3254,7 +3450,7 @@
       <c r="Q23" s="31">
         <v>10</v>
       </c>
-      <c r="R23" s="102">
+      <c r="R23" s="101">
         <v>3</v>
       </c>
       <c r="S23" s="9" t="s">
@@ -3267,7 +3463,7 @@
     </row>
     <row r="24" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="43"/>
-      <c r="B24" s="100"/>
+      <c r="B24" s="102"/>
       <c r="C24" s="9" t="s">
         <v>50</v>
       </c>
@@ -3275,15 +3471,15 @@
         <v>354</v>
       </c>
       <c r="E24" s="43"/>
-      <c r="F24" s="102"/>
-      <c r="G24" s="102"/>
+      <c r="F24" s="101"/>
+      <c r="G24" s="101"/>
       <c r="H24" s="9" t="s">
         <v>300</v>
       </c>
       <c r="I24" s="31">
         <v>14</v>
       </c>
-      <c r="J24" s="102"/>
+      <c r="J24" s="101"/>
       <c r="K24" s="9" t="s">
         <v>305</v>
       </c>
@@ -3291,15 +3487,15 @@
         <v>15</v>
       </c>
       <c r="M24" s="14"/>
-      <c r="N24" s="102"/>
-      <c r="O24" s="102"/>
+      <c r="N24" s="101"/>
+      <c r="O24" s="101"/>
       <c r="P24" s="9" t="s">
         <v>293</v>
       </c>
       <c r="Q24" s="31">
         <v>14</v>
       </c>
-      <c r="R24" s="102"/>
+      <c r="R24" s="101"/>
       <c r="S24" s="9" t="s">
         <v>305</v>
       </c>
@@ -3310,7 +3506,7 @@
     </row>
     <row r="25" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="43"/>
-      <c r="B25" s="101">
+      <c r="B25" s="103">
         <v>0.4861111111111111</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -3320,10 +3516,10 @@
         <v>24</v>
       </c>
       <c r="E25" s="43"/>
-      <c r="F25" s="103" t="s">
+      <c r="F25" s="100" t="s">
         <v>359</v>
       </c>
-      <c r="G25" s="103">
+      <c r="G25" s="100">
         <v>2</v>
       </c>
       <c r="H25" s="3" t="s">
@@ -3332,7 +3528,7 @@
       <c r="I25" s="33">
         <v>11</v>
       </c>
-      <c r="J25" s="103">
+      <c r="J25" s="100">
         <v>3</v>
       </c>
       <c r="K25" s="3" t="s">
@@ -3342,10 +3538,10 @@
         <v>30</v>
       </c>
       <c r="M25" s="14"/>
-      <c r="N25" s="103" t="s">
+      <c r="N25" s="100" t="s">
         <v>330</v>
       </c>
-      <c r="O25" s="103">
+      <c r="O25" s="100">
         <v>1</v>
       </c>
       <c r="P25" s="3" t="s">
@@ -3354,7 +3550,7 @@
       <c r="Q25" s="33">
         <v>14</v>
       </c>
-      <c r="R25" s="103">
+      <c r="R25" s="100">
         <v>2</v>
       </c>
       <c r="S25" s="3" t="s">
@@ -3367,21 +3563,21 @@
     </row>
     <row r="26" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="43"/>
-      <c r="B26" s="101"/>
+      <c r="B26" s="103"/>
       <c r="C26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="43"/>
-      <c r="F26" s="103"/>
-      <c r="G26" s="103"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
       <c r="H26" s="3" t="s">
         <v>298</v>
       </c>
       <c r="I26" s="33">
         <v>18</v>
       </c>
-      <c r="J26" s="103"/>
+      <c r="J26" s="100"/>
       <c r="K26" s="3" t="s">
         <v>304</v>
       </c>
@@ -3389,22 +3585,22 @@
         <v>9</v>
       </c>
       <c r="M26" s="14"/>
-      <c r="N26" s="103"/>
-      <c r="O26" s="103"/>
+      <c r="N26" s="100"/>
+      <c r="O26" s="100"/>
       <c r="P26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="Q26" s="33">
         <v>7</v>
       </c>
-      <c r="R26" s="103"/>
+      <c r="R26" s="100"/>
       <c r="S26" s="3"/>
       <c r="T26" s="33"/>
       <c r="U26" s="14"/>
     </row>
     <row r="27" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="43"/>
-      <c r="B27" s="100">
+      <c r="B27" s="102">
         <v>0.52083333333333337</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -3414,10 +3610,10 @@
         <v>54</v>
       </c>
       <c r="E27" s="43"/>
-      <c r="F27" s="102" t="s">
+      <c r="F27" s="101" t="s">
         <v>358</v>
       </c>
-      <c r="G27" s="102">
+      <c r="G27" s="101">
         <v>3</v>
       </c>
       <c r="H27" s="9" t="s">
@@ -3426,7 +3622,7 @@
       <c r="I27" s="31">
         <v>23</v>
       </c>
-      <c r="J27" s="102">
+      <c r="J27" s="101">
         <v>3</v>
       </c>
       <c r="K27" s="9" t="s">
@@ -3436,10 +3632,10 @@
         <v>21</v>
       </c>
       <c r="M27" s="14"/>
-      <c r="N27" s="102" t="s">
+      <c r="N27" s="101" t="s">
         <v>331</v>
       </c>
-      <c r="O27" s="102">
+      <c r="O27" s="101">
         <v>2</v>
       </c>
       <c r="P27" s="9" t="s">
@@ -3448,7 +3644,7 @@
       <c r="Q27" s="31">
         <v>20</v>
       </c>
-      <c r="R27" s="102">
+      <c r="R27" s="101">
         <v>2</v>
       </c>
       <c r="S27" s="9" t="s">
@@ -3461,7 +3657,7 @@
     </row>
     <row r="28" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="43"/>
-      <c r="B28" s="100"/>
+      <c r="B28" s="102"/>
       <c r="C28" s="9" t="s">
         <v>69</v>
       </c>
@@ -3469,15 +3665,15 @@
         <v>53</v>
       </c>
       <c r="E28" s="43"/>
-      <c r="F28" s="102"/>
-      <c r="G28" s="102"/>
+      <c r="F28" s="101"/>
+      <c r="G28" s="101"/>
       <c r="H28" s="9" t="s">
         <v>308</v>
       </c>
       <c r="I28" s="31">
         <v>28</v>
       </c>
-      <c r="J28" s="102"/>
+      <c r="J28" s="101"/>
       <c r="K28" s="9" t="s">
         <v>302</v>
       </c>
@@ -3485,22 +3681,22 @@
         <v>14</v>
       </c>
       <c r="M28" s="14"/>
-      <c r="N28" s="102"/>
-      <c r="O28" s="102"/>
+      <c r="N28" s="101"/>
+      <c r="O28" s="101"/>
       <c r="P28" s="9" t="s">
         <v>342</v>
       </c>
       <c r="Q28" s="31">
         <v>8</v>
       </c>
-      <c r="R28" s="102"/>
+      <c r="R28" s="101"/>
       <c r="S28" s="9"/>
       <c r="T28" s="31"/>
       <c r="U28" s="14"/>
     </row>
     <row r="29" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="43"/>
-      <c r="B29" s="101">
+      <c r="B29" s="103">
         <v>0.59722222222222221</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -3510,10 +3706,10 @@
         <v>28</v>
       </c>
       <c r="E29" s="43"/>
-      <c r="F29" s="103" t="s">
+      <c r="F29" s="100" t="s">
         <v>323</v>
       </c>
-      <c r="G29" s="103">
+      <c r="G29" s="100">
         <v>1</v>
       </c>
       <c r="H29" s="3" t="s">
@@ -3522,7 +3718,7 @@
       <c r="I29" s="33">
         <v>10</v>
       </c>
-      <c r="J29" s="103">
+      <c r="J29" s="100">
         <v>3</v>
       </c>
       <c r="K29" s="3" t="s">
@@ -3532,10 +3728,10 @@
         <v>19</v>
       </c>
       <c r="M29" s="14"/>
-      <c r="N29" s="103" t="s">
+      <c r="N29" s="100" t="s">
         <v>332</v>
       </c>
-      <c r="O29" s="103">
+      <c r="O29" s="100">
         <v>3</v>
       </c>
       <c r="P29" s="3" t="s">
@@ -3544,7 +3740,7 @@
       <c r="Q29" s="33">
         <v>23</v>
       </c>
-      <c r="R29" s="103">
+      <c r="R29" s="100">
         <v>3</v>
       </c>
       <c r="S29" s="3" t="s">
@@ -3557,21 +3753,21 @@
     </row>
     <row r="30" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="43"/>
-      <c r="B30" s="101"/>
+      <c r="B30" s="103"/>
       <c r="C30" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="43"/>
-      <c r="F30" s="103"/>
-      <c r="G30" s="103"/>
+      <c r="F30" s="100"/>
+      <c r="G30" s="100"/>
       <c r="H30" s="3" t="s">
         <v>293</v>
       </c>
       <c r="I30" s="33">
         <v>14</v>
       </c>
-      <c r="J30" s="103"/>
+      <c r="J30" s="100"/>
       <c r="K30" s="3" t="s">
         <v>296</v>
       </c>
@@ -3579,15 +3775,15 @@
         <v>35</v>
       </c>
       <c r="M30" s="14"/>
-      <c r="N30" s="103"/>
-      <c r="O30" s="103"/>
+      <c r="N30" s="100"/>
+      <c r="O30" s="100"/>
       <c r="P30" s="3" t="s">
         <v>308</v>
       </c>
       <c r="Q30" s="33">
         <v>28</v>
       </c>
-      <c r="R30" s="103"/>
+      <c r="R30" s="100"/>
       <c r="S30" s="3" t="s">
         <v>304</v>
       </c>
@@ -3598,7 +3794,7 @@
     </row>
     <row r="31" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="43"/>
-      <c r="B31" s="100">
+      <c r="B31" s="102">
         <v>0.60416666666666663</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -3608,10 +3804,10 @@
         <v>30</v>
       </c>
       <c r="E31" s="43"/>
-      <c r="F31" s="102" t="s">
+      <c r="F31" s="101" t="s">
         <v>324</v>
       </c>
-      <c r="G31" s="102">
+      <c r="G31" s="101">
         <v>2</v>
       </c>
       <c r="H31" s="9" t="s">
@@ -3620,7 +3816,7 @@
       <c r="I31" s="31">
         <v>20</v>
       </c>
-      <c r="J31" s="102">
+      <c r="J31" s="101">
         <v>2</v>
       </c>
       <c r="K31" s="9" t="s">
@@ -3630,10 +3826,10 @@
         <v>15</v>
       </c>
       <c r="M31" s="14"/>
-      <c r="N31" s="102" t="s">
+      <c r="N31" s="101" t="s">
         <v>333</v>
       </c>
-      <c r="O31" s="102">
+      <c r="O31" s="101">
         <v>3</v>
       </c>
       <c r="P31" s="9" t="s">
@@ -3642,7 +3838,7 @@
       <c r="Q31" s="31">
         <v>19</v>
       </c>
-      <c r="R31" s="102">
+      <c r="R31" s="101">
         <v>2</v>
       </c>
       <c r="S31" s="9" t="s">
@@ -3655,21 +3851,21 @@
     </row>
     <row r="32" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="43"/>
-      <c r="B32" s="100"/>
+      <c r="B32" s="102"/>
       <c r="C32" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="43"/>
-      <c r="F32" s="102"/>
-      <c r="G32" s="102"/>
+      <c r="F32" s="101"/>
+      <c r="G32" s="101"/>
       <c r="H32" s="9" t="s">
         <v>342</v>
       </c>
       <c r="I32" s="31">
         <v>8</v>
       </c>
-      <c r="J32" s="102"/>
+      <c r="J32" s="101"/>
       <c r="K32" s="9" t="s">
         <v>357</v>
       </c>
@@ -3677,15 +3873,15 @@
         <v>12</v>
       </c>
       <c r="M32" s="14"/>
-      <c r="N32" s="102"/>
-      <c r="O32" s="102"/>
+      <c r="N32" s="101"/>
+      <c r="O32" s="101"/>
       <c r="P32" s="9" t="s">
         <v>296</v>
       </c>
       <c r="Q32" s="31">
         <v>35</v>
       </c>
-      <c r="R32" s="102"/>
+      <c r="R32" s="101"/>
       <c r="S32" s="9" t="s">
         <v>300</v>
       </c>
@@ -3700,10 +3896,10 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="43"/>
-      <c r="F33" s="103" t="s">
+      <c r="F33" s="100" t="s">
         <v>325</v>
       </c>
-      <c r="G33" s="103">
+      <c r="G33" s="100">
         <v>3</v>
       </c>
       <c r="H33" s="3" t="s">
@@ -3712,7 +3908,7 @@
       <c r="I33" s="33">
         <v>25</v>
       </c>
-      <c r="J33" s="103">
+      <c r="J33" s="100">
         <v>3</v>
       </c>
       <c r="K33" s="3" t="s">
@@ -3722,10 +3918,10 @@
         <v>36</v>
       </c>
       <c r="M33" s="14"/>
-      <c r="N33" s="103" t="s">
+      <c r="N33" s="100" t="s">
         <v>334</v>
       </c>
-      <c r="O33" s="103">
+      <c r="O33" s="100">
         <v>3</v>
       </c>
       <c r="P33" s="3" t="s">
@@ -3734,7 +3930,7 @@
       <c r="Q33" s="33">
         <v>21</v>
       </c>
-      <c r="R33" s="103">
+      <c r="R33" s="100">
         <v>3</v>
       </c>
       <c r="S33" s="3" t="s">
@@ -3751,27 +3947,27 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="43"/>
-      <c r="F34" s="103"/>
-      <c r="G34" s="103"/>
+      <c r="F34" s="100"/>
+      <c r="G34" s="100"/>
       <c r="H34" s="3" t="s">
         <v>312</v>
       </c>
       <c r="I34" s="33">
         <v>43</v>
       </c>
-      <c r="J34" s="103"/>
+      <c r="J34" s="100"/>
       <c r="K34" s="3"/>
       <c r="L34" s="33"/>
       <c r="M34" s="14"/>
-      <c r="N34" s="103"/>
-      <c r="O34" s="103"/>
+      <c r="N34" s="100"/>
+      <c r="O34" s="100"/>
       <c r="P34" s="3" t="s">
         <v>310</v>
       </c>
       <c r="Q34" s="33">
         <v>31</v>
       </c>
-      <c r="R34" s="103"/>
+      <c r="R34" s="100"/>
       <c r="S34" s="3" t="s">
         <v>288</v>
       </c>
@@ -3786,10 +3982,10 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="11"/>
-      <c r="F35" s="102" t="s">
+      <c r="F35" s="101" t="s">
         <v>326</v>
       </c>
-      <c r="G35" s="102">
+      <c r="G35" s="101">
         <v>3</v>
       </c>
       <c r="H35" s="9" t="s">
@@ -3798,7 +3994,7 @@
       <c r="I35" s="31">
         <v>10</v>
       </c>
-      <c r="J35" s="102">
+      <c r="J35" s="101">
         <v>3</v>
       </c>
       <c r="K35" s="9" t="s">
@@ -3808,10 +4004,10 @@
         <v>40</v>
       </c>
       <c r="M35" s="14"/>
-      <c r="N35" s="102" t="s">
+      <c r="N35" s="101" t="s">
         <v>335</v>
       </c>
-      <c r="O35" s="102">
+      <c r="O35" s="101">
         <v>3</v>
       </c>
       <c r="P35" s="9" t="s">
@@ -3820,7 +4016,7 @@
       <c r="Q35" s="31">
         <v>25</v>
       </c>
-      <c r="R35" s="102">
+      <c r="R35" s="101">
         <v>3</v>
       </c>
       <c r="S35" s="9" t="s">
@@ -3837,27 +4033,27 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="11"/>
-      <c r="F36" s="102"/>
-      <c r="G36" s="102"/>
+      <c r="F36" s="101"/>
+      <c r="G36" s="101"/>
       <c r="H36" s="9" t="s">
         <v>274</v>
       </c>
       <c r="I36" s="31">
         <v>28</v>
       </c>
-      <c r="J36" s="102"/>
+      <c r="J36" s="101"/>
       <c r="K36" s="9"/>
       <c r="L36" s="31"/>
       <c r="M36" s="14"/>
-      <c r="N36" s="102"/>
-      <c r="O36" s="102"/>
+      <c r="N36" s="101"/>
+      <c r="O36" s="101"/>
       <c r="P36" s="9" t="s">
         <v>312</v>
       </c>
       <c r="Q36" s="31">
         <v>43</v>
       </c>
-      <c r="R36" s="102"/>
+      <c r="R36" s="101"/>
       <c r="S36" s="9" t="s">
         <v>134</v>
       </c>
@@ -6086,85 +6282,20 @@
     </row>
   </sheetData>
   <mergeCells count="117">
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="N35:N36"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="J35:J36"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="N33:N34"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="N29:N30"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="N31:N32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="O31:O32"/>
-    <mergeCell ref="O33:O34"/>
-    <mergeCell ref="J31:J32"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="O29:O30"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O22"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B15:B16"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
@@ -6189,20 +6320,85 @@
     <mergeCell ref="R27:R28"/>
     <mergeCell ref="O35:O36"/>
     <mergeCell ref="J3:J4"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="O31:O32"/>
+    <mergeCell ref="O33:O34"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="O29:O30"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="N35:N36"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="N33:N34"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="N29:N30"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="N31:N32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="J13:J14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6213,7 +6409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -6337,10 +6533,10 @@
       <c r="K2" s="45">
         <v>1</v>
       </c>
-      <c r="L2" s="108" t="s">
+      <c r="L2" s="104" t="s">
         <v>362</v>
       </c>
-      <c r="M2" s="109" t="s">
+      <c r="M2" s="105" t="s">
         <v>177</v>
       </c>
       <c r="N2" s="95" t="str">
@@ -6404,8 +6600,8 @@
       <c r="K3" s="45">
         <v>1</v>
       </c>
-      <c r="L3" s="108"/>
-      <c r="M3" s="109"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="105"/>
       <c r="N3" s="95" t="str">
         <f t="shared" ref="N3:N9" si="3">CONCATENATE(B3," ", C3)</f>
         <v>Jim Clark</v>
@@ -6467,8 +6663,8 @@
       <c r="K4" s="45">
         <v>1</v>
       </c>
-      <c r="L4" s="108"/>
-      <c r="M4" s="109"/>
+      <c r="L4" s="104"/>
+      <c r="M4" s="105"/>
       <c r="N4" s="95" t="str">
         <f t="shared" si="3"/>
         <v>Aaron Wald</v>
@@ -6530,8 +6726,8 @@
       <c r="K5" s="45">
         <v>1</v>
       </c>
-      <c r="L5" s="108"/>
-      <c r="M5" s="109"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="105"/>
       <c r="N5" s="95" t="str">
         <f t="shared" si="3"/>
         <v>Chris Callahan</v>
@@ -6593,8 +6789,8 @@
       <c r="K6" s="45">
         <v>1</v>
       </c>
-      <c r="L6" s="108"/>
-      <c r="M6" s="109"/>
+      <c r="L6" s="104"/>
+      <c r="M6" s="105"/>
       <c r="N6" s="95" t="str">
         <f t="shared" si="3"/>
         <v>Todd Bodine</v>
@@ -6658,8 +6854,8 @@
       <c r="K7" s="45">
         <v>1</v>
       </c>
-      <c r="L7" s="108"/>
-      <c r="M7" s="109"/>
+      <c r="L7" s="104"/>
+      <c r="M7" s="105"/>
       <c r="N7" s="95" t="str">
         <f t="shared" si="3"/>
         <v>Doug Wald</v>
@@ -6706,8 +6902,8 @@
       <c r="K8" s="45">
         <v>1</v>
       </c>
-      <c r="L8" s="108"/>
-      <c r="M8" s="109"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="105"/>
       <c r="N8" s="95" t="str">
         <f t="shared" si="3"/>
         <v>Andy Ness</v>
@@ -6754,8 +6950,8 @@
       <c r="K9" s="45">
         <v>1</v>
       </c>
-      <c r="L9" s="108"/>
-      <c r="M9" s="109"/>
+      <c r="L9" s="104"/>
+      <c r="M9" s="105"/>
       <c r="N9" s="95" t="str">
         <f t="shared" si="3"/>
         <v>Steve Wald</v>
@@ -6802,10 +6998,10 @@
       <c r="K10" s="46">
         <v>2</v>
       </c>
-      <c r="L10" s="106" t="s">
+      <c r="L10" s="108" t="s">
         <v>363</v>
       </c>
-      <c r="M10" s="107" t="s">
+      <c r="M10" s="109" t="s">
         <v>195</v>
       </c>
       <c r="N10" s="96" t="str">
@@ -6854,8 +7050,8 @@
       <c r="K11" s="46">
         <v>2</v>
       </c>
-      <c r="L11" s="106"/>
-      <c r="M11" s="107"/>
+      <c r="L11" s="108"/>
+      <c r="M11" s="109"/>
       <c r="N11" s="96" t="str">
         <f t="shared" ref="N11:N13" si="5">CONCATENATE(B11," ", C11)</f>
         <v>Jeff Wald</v>
@@ -6902,8 +7098,8 @@
       <c r="K12" s="46">
         <v>2</v>
       </c>
-      <c r="L12" s="106"/>
-      <c r="M12" s="107"/>
+      <c r="L12" s="108"/>
+      <c r="M12" s="109"/>
       <c r="N12" s="96" t="str">
         <f t="shared" si="5"/>
         <v>Wayne Podolak</v>
@@ -6950,8 +7146,8 @@
       <c r="K13" s="46">
         <v>2</v>
       </c>
-      <c r="L13" s="106"/>
-      <c r="M13" s="107"/>
+      <c r="L13" s="108"/>
+      <c r="M13" s="109"/>
       <c r="N13" s="96" t="str">
         <f t="shared" si="5"/>
         <v>Bob Holso</v>
@@ -6996,8 +7192,8 @@
         <v>26</v>
       </c>
       <c r="K14" s="93"/>
-      <c r="L14" s="106"/>
-      <c r="M14" s="107"/>
+      <c r="L14" s="108"/>
+      <c r="M14" s="109"/>
       <c r="N14" s="97"/>
       <c r="O14" s="97"/>
     </row>
@@ -7038,8 +7234,8 @@
       <c r="K15" s="46">
         <v>2</v>
       </c>
-      <c r="L15" s="106"/>
-      <c r="M15" s="107"/>
+      <c r="L15" s="108"/>
+      <c r="M15" s="109"/>
       <c r="N15" s="96" t="str">
         <f t="shared" ref="N15" si="7">CONCATENATE(B15," ", C15)</f>
         <v>Myron Irwin</v>
@@ -7084,8 +7280,8 @@
         <v>28</v>
       </c>
       <c r="K16" s="93"/>
-      <c r="L16" s="106"/>
-      <c r="M16" s="107"/>
+      <c r="L16" s="108"/>
+      <c r="M16" s="109"/>
       <c r="N16" s="97"/>
       <c r="O16" s="97"/>
     </row>
@@ -7124,8 +7320,8 @@
         <v>28</v>
       </c>
       <c r="K17" s="93"/>
-      <c r="L17" s="106"/>
-      <c r="M17" s="107"/>
+      <c r="L17" s="108"/>
+      <c r="M17" s="109"/>
       <c r="N17" s="97"/>
       <c r="O17" s="97"/>
     </row>
@@ -7166,8 +7362,8 @@
       <c r="K18" s="46">
         <v>2</v>
       </c>
-      <c r="L18" s="106"/>
-      <c r="M18" s="107"/>
+      <c r="L18" s="108"/>
+      <c r="M18" s="109"/>
       <c r="N18" s="96" t="str">
         <f t="shared" ref="N18:N21" si="9">CONCATENATE(B18," ", C18)</f>
         <v>Mike Stork</v>
@@ -7214,8 +7410,8 @@
       <c r="K19" s="46">
         <v>2</v>
       </c>
-      <c r="L19" s="106"/>
-      <c r="M19" s="107"/>
+      <c r="L19" s="108"/>
+      <c r="M19" s="109"/>
       <c r="N19" s="96" t="str">
         <f t="shared" si="9"/>
         <v>Steve Francis</v>
@@ -7262,8 +7458,8 @@
       <c r="K20" s="46">
         <v>2</v>
       </c>
-      <c r="L20" s="106"/>
-      <c r="M20" s="107"/>
+      <c r="L20" s="108"/>
+      <c r="M20" s="109"/>
       <c r="N20" s="96" t="str">
         <f t="shared" si="9"/>
         <v>Joe Bichler</v>
@@ -7310,10 +7506,10 @@
       <c r="K21" s="47">
         <v>3</v>
       </c>
-      <c r="L21" s="104" t="s">
+      <c r="L21" s="106" t="s">
         <v>364</v>
       </c>
-      <c r="M21" s="104" t="s">
+      <c r="M21" s="106" t="s">
         <v>224</v>
       </c>
       <c r="N21" s="98" t="str">
@@ -7362,8 +7558,8 @@
       <c r="K22" s="47">
         <v>3</v>
       </c>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
+      <c r="L22" s="106"/>
+      <c r="M22" s="106"/>
       <c r="N22" s="98" t="str">
         <f t="shared" ref="N22:N23" si="11">CONCATENATE(B22," ", C22)</f>
         <v>Jon Gies</v>
@@ -7410,8 +7606,8 @@
       <c r="K23" s="47">
         <v>3</v>
       </c>
-      <c r="L23" s="104"/>
-      <c r="M23" s="104"/>
+      <c r="L23" s="106"/>
+      <c r="M23" s="106"/>
       <c r="N23" s="98" t="str">
         <f t="shared" si="11"/>
         <v>KT Thayer</v>
@@ -7458,8 +7654,8 @@
       <c r="K24" s="47">
         <v>3</v>
       </c>
-      <c r="L24" s="104"/>
-      <c r="M24" s="104"/>
+      <c r="L24" s="106"/>
+      <c r="M24" s="106"/>
       <c r="N24" s="98" t="str">
         <f t="shared" ref="N24:N27" si="13">CONCATENATE(B24," ", C24)</f>
         <v>Joel Van Dyk</v>
@@ -7506,8 +7702,8 @@
       <c r="K25" s="47">
         <v>3</v>
       </c>
-      <c r="L25" s="104"/>
-      <c r="M25" s="104"/>
+      <c r="L25" s="106"/>
+      <c r="M25" s="106"/>
       <c r="N25" s="98" t="str">
         <f t="shared" si="13"/>
         <v>Dewey Wald</v>
@@ -7554,8 +7750,8 @@
       <c r="K26" s="47">
         <v>3</v>
       </c>
-      <c r="L26" s="104"/>
-      <c r="M26" s="104"/>
+      <c r="L26" s="106"/>
+      <c r="M26" s="106"/>
       <c r="N26" s="98" t="str">
         <f t="shared" si="13"/>
         <v>Derek Gulbransen</v>
@@ -7602,8 +7798,8 @@
       <c r="K27" s="47">
         <v>3</v>
       </c>
-      <c r="L27" s="104"/>
-      <c r="M27" s="104"/>
+      <c r="L27" s="106"/>
+      <c r="M27" s="106"/>
       <c r="N27" s="98" t="str">
         <f t="shared" si="13"/>
         <v>Brad Epker</v>
@@ -7650,10 +7846,10 @@
       <c r="K28" s="48">
         <v>4</v>
       </c>
-      <c r="L28" s="105" t="s">
+      <c r="L28" s="107" t="s">
         <v>365</v>
       </c>
-      <c r="M28" s="105" t="s">
+      <c r="M28" s="107" t="s">
         <v>234</v>
       </c>
       <c r="N28" s="99" t="str">
@@ -7702,8 +7898,8 @@
       <c r="K29" s="48">
         <v>4</v>
       </c>
-      <c r="L29" s="105"/>
-      <c r="M29" s="105"/>
+      <c r="L29" s="107"/>
+      <c r="M29" s="107"/>
       <c r="N29" s="99" t="str">
         <f t="shared" ref="N29:N31" si="17">CONCATENATE(B29," ", C29)</f>
         <v>Dwane Liuska</v>
@@ -7750,8 +7946,8 @@
       <c r="K30" s="48">
         <v>4</v>
       </c>
-      <c r="L30" s="105"/>
-      <c r="M30" s="105"/>
+      <c r="L30" s="107"/>
+      <c r="M30" s="107"/>
       <c r="N30" s="99" t="str">
         <f t="shared" si="17"/>
         <v>Bob Cruzan</v>
@@ -7798,8 +7994,8 @@
       <c r="K31" s="48">
         <v>4</v>
       </c>
-      <c r="L31" s="105"/>
-      <c r="M31" s="105"/>
+      <c r="L31" s="107"/>
+      <c r="M31" s="107"/>
       <c r="N31" s="99" t="str">
         <f t="shared" si="17"/>
         <v>Garth Billsten</v>
@@ -7846,8 +8042,8 @@
       <c r="K32" s="48">
         <v>4</v>
       </c>
-      <c r="L32" s="105"/>
-      <c r="M32" s="105"/>
+      <c r="L32" s="107"/>
+      <c r="M32" s="107"/>
       <c r="N32" s="99" t="str">
         <f t="shared" ref="N32:N34" si="19">CONCATENATE(B32," ", C32)</f>
         <v>Andy Podolak</v>
@@ -7894,8 +8090,8 @@
       <c r="K33" s="48">
         <v>4</v>
       </c>
-      <c r="L33" s="105"/>
-      <c r="M33" s="105"/>
+      <c r="L33" s="107"/>
+      <c r="M33" s="107"/>
       <c r="N33" s="99" t="str">
         <f t="shared" si="19"/>
         <v>Guy Rasmussen</v>
@@ -7942,8 +8138,8 @@
       <c r="K34" s="48">
         <v>4</v>
       </c>
-      <c r="L34" s="105"/>
-      <c r="M34" s="105"/>
+      <c r="L34" s="107"/>
+      <c r="M34" s="107"/>
       <c r="N34" s="99" t="str">
         <f t="shared" si="19"/>
         <v>Laura Roseleip</v>
@@ -11751,4 +11947,2455 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA16" sqref="AA16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" t="s">
+        <v>414</v>
+      </c>
+      <c r="E1" t="s">
+        <v>415</v>
+      </c>
+      <c r="F1" t="s">
+        <v>416</v>
+      </c>
+      <c r="G1" t="s">
+        <v>417</v>
+      </c>
+      <c r="H1" t="s">
+        <v>418</v>
+      </c>
+      <c r="I1" t="s">
+        <v>419</v>
+      </c>
+      <c r="J1" t="s">
+        <v>420</v>
+      </c>
+      <c r="K1" t="s">
+        <v>421</v>
+      </c>
+      <c r="L1" t="s">
+        <v>418</v>
+      </c>
+      <c r="M1" t="s">
+        <v>419</v>
+      </c>
+      <c r="N1" t="s">
+        <v>420</v>
+      </c>
+      <c r="O1" t="s">
+        <v>416</v>
+      </c>
+      <c r="P1" t="s">
+        <v>417</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>418</v>
+      </c>
+      <c r="R1" t="s">
+        <v>419</v>
+      </c>
+      <c r="S1" t="s">
+        <v>420</v>
+      </c>
+      <c r="T1" t="s">
+        <v>421</v>
+      </c>
+      <c r="U1" t="s">
+        <v>418</v>
+      </c>
+      <c r="V1" t="s">
+        <v>419</v>
+      </c>
+      <c r="W1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="110">
+        <v>1</v>
+      </c>
+      <c r="B2" s="111" t="s">
+        <v>422</v>
+      </c>
+      <c r="C2" s="110">
+        <v>91</v>
+      </c>
+      <c r="D2" s="110">
+        <v>101</v>
+      </c>
+      <c r="E2" s="110">
+        <v>192</v>
+      </c>
+      <c r="F2" s="112" t="s">
+        <v>263</v>
+      </c>
+      <c r="G2" s="110">
+        <v>69</v>
+      </c>
+      <c r="H2" s="110">
+        <v>2</v>
+      </c>
+      <c r="I2" s="110">
+        <v>67</v>
+      </c>
+      <c r="J2" s="110">
+        <v>69</v>
+      </c>
+      <c r="K2" s="110">
+        <v>71</v>
+      </c>
+      <c r="L2" s="110">
+        <v>2</v>
+      </c>
+      <c r="M2" s="110">
+        <v>69</v>
+      </c>
+      <c r="N2" s="110">
+        <v>71</v>
+      </c>
+      <c r="O2" s="112" t="s">
+        <v>352</v>
+      </c>
+      <c r="P2" s="110">
+        <v>76</v>
+      </c>
+      <c r="Q2" s="110">
+        <v>9</v>
+      </c>
+      <c r="R2" s="110">
+        <v>67</v>
+      </c>
+      <c r="S2" s="110">
+        <v>76</v>
+      </c>
+      <c r="T2" s="110">
+        <v>82</v>
+      </c>
+      <c r="U2" s="110">
+        <v>9</v>
+      </c>
+      <c r="V2" s="110">
+        <v>73</v>
+      </c>
+      <c r="W2" s="110">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="110">
+        <v>1</v>
+      </c>
+      <c r="B3" s="111" t="s">
+        <v>423</v>
+      </c>
+      <c r="C3" s="110">
+        <v>92</v>
+      </c>
+      <c r="D3" s="110">
+        <v>100</v>
+      </c>
+      <c r="E3" s="110">
+        <v>192</v>
+      </c>
+      <c r="F3" s="112" t="s">
+        <v>278</v>
+      </c>
+      <c r="G3" s="110">
+        <v>78</v>
+      </c>
+      <c r="H3" s="110">
+        <v>12</v>
+      </c>
+      <c r="I3" s="110">
+        <v>66</v>
+      </c>
+      <c r="J3" s="110">
+        <v>78</v>
+      </c>
+      <c r="K3" s="110">
+        <v>81</v>
+      </c>
+      <c r="L3" s="110">
+        <v>12</v>
+      </c>
+      <c r="M3" s="110">
+        <v>69</v>
+      </c>
+      <c r="N3" s="110">
+        <v>81</v>
+      </c>
+      <c r="O3" s="112" t="s">
+        <v>277</v>
+      </c>
+      <c r="P3" s="110">
+        <v>80</v>
+      </c>
+      <c r="Q3" s="110">
+        <v>8</v>
+      </c>
+      <c r="R3" s="110">
+        <v>72</v>
+      </c>
+      <c r="S3" s="110">
+        <v>80</v>
+      </c>
+      <c r="T3" s="110">
+        <v>79</v>
+      </c>
+      <c r="U3" s="110">
+        <v>8</v>
+      </c>
+      <c r="V3" s="110">
+        <v>71</v>
+      </c>
+      <c r="W3" s="110">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="110">
+        <v>1</v>
+      </c>
+      <c r="B4" s="111" t="s">
+        <v>424</v>
+      </c>
+      <c r="C4" s="110">
+        <v>96</v>
+      </c>
+      <c r="D4" s="110">
+        <v>109</v>
+      </c>
+      <c r="E4" s="110">
+        <v>205</v>
+      </c>
+      <c r="F4" s="112" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="110">
+        <v>74</v>
+      </c>
+      <c r="H4" s="110">
+        <v>7</v>
+      </c>
+      <c r="I4" s="110">
+        <v>67</v>
+      </c>
+      <c r="J4" s="110">
+        <v>74</v>
+      </c>
+      <c r="K4" s="110">
+        <v>85</v>
+      </c>
+      <c r="L4" s="110">
+        <v>7</v>
+      </c>
+      <c r="M4" s="110">
+        <v>78</v>
+      </c>
+      <c r="N4" s="110">
+        <v>85</v>
+      </c>
+      <c r="O4" s="112" t="s">
+        <v>292</v>
+      </c>
+      <c r="P4" s="110">
+        <v>91</v>
+      </c>
+      <c r="Q4" s="110">
+        <v>14</v>
+      </c>
+      <c r="R4" s="110">
+        <v>77</v>
+      </c>
+      <c r="S4" s="110">
+        <v>90</v>
+      </c>
+      <c r="T4" s="110">
+        <v>88</v>
+      </c>
+      <c r="U4" s="110">
+        <v>14</v>
+      </c>
+      <c r="V4" s="110">
+        <v>74</v>
+      </c>
+      <c r="W4" s="110">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="110">
+        <v>1</v>
+      </c>
+      <c r="B5" s="111" t="s">
+        <v>425</v>
+      </c>
+      <c r="C5" s="110">
+        <v>101</v>
+      </c>
+      <c r="D5" s="110">
+        <v>105</v>
+      </c>
+      <c r="E5" s="110">
+        <v>206</v>
+      </c>
+      <c r="F5" s="112" t="s">
+        <v>262</v>
+      </c>
+      <c r="G5" s="110">
+        <v>89</v>
+      </c>
+      <c r="H5" s="110">
+        <v>12</v>
+      </c>
+      <c r="I5" s="110">
+        <v>77</v>
+      </c>
+      <c r="J5" s="110">
+        <v>89</v>
+      </c>
+      <c r="K5" s="110">
+        <v>87</v>
+      </c>
+      <c r="L5" s="110">
+        <v>12</v>
+      </c>
+      <c r="M5" s="110">
+        <v>75</v>
+      </c>
+      <c r="N5" s="110">
+        <v>86</v>
+      </c>
+      <c r="O5" s="112" t="s">
+        <v>261</v>
+      </c>
+      <c r="P5" s="110">
+        <v>74</v>
+      </c>
+      <c r="Q5" s="110">
+        <v>5</v>
+      </c>
+      <c r="R5" s="110">
+        <v>69</v>
+      </c>
+      <c r="S5" s="110">
+        <v>74</v>
+      </c>
+      <c r="T5" s="110">
+        <v>72</v>
+      </c>
+      <c r="U5" s="110">
+        <v>5</v>
+      </c>
+      <c r="V5" s="110">
+        <v>67</v>
+      </c>
+      <c r="W5" s="110">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="110">
+        <v>1</v>
+      </c>
+      <c r="B6" s="111" t="s">
+        <v>426</v>
+      </c>
+      <c r="C6" s="110">
+        <v>99</v>
+      </c>
+      <c r="D6" s="110">
+        <v>109</v>
+      </c>
+      <c r="E6" s="110">
+        <v>208</v>
+      </c>
+      <c r="F6" s="112" t="s">
+        <v>259</v>
+      </c>
+      <c r="G6" s="110">
+        <v>92</v>
+      </c>
+      <c r="H6" s="110">
+        <v>16</v>
+      </c>
+      <c r="I6" s="110">
+        <v>76</v>
+      </c>
+      <c r="J6" s="110">
+        <v>91</v>
+      </c>
+      <c r="K6" s="110">
+        <v>95</v>
+      </c>
+      <c r="L6" s="110">
+        <v>16</v>
+      </c>
+      <c r="M6" s="110">
+        <v>79</v>
+      </c>
+      <c r="N6" s="110">
+        <v>93</v>
+      </c>
+      <c r="O6" s="112" t="s">
+        <v>260</v>
+      </c>
+      <c r="P6" s="110">
+        <v>76</v>
+      </c>
+      <c r="Q6" s="110">
+        <v>7</v>
+      </c>
+      <c r="R6" s="110">
+        <v>69</v>
+      </c>
+      <c r="S6" s="110">
+        <v>76</v>
+      </c>
+      <c r="T6" s="110">
+        <v>78</v>
+      </c>
+      <c r="U6" s="110">
+        <v>7</v>
+      </c>
+      <c r="V6" s="110">
+        <v>71</v>
+      </c>
+      <c r="W6" s="110">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="110">
+        <v>1</v>
+      </c>
+      <c r="B7" s="111" t="s">
+        <v>427</v>
+      </c>
+      <c r="C7" s="110">
+        <v>104</v>
+      </c>
+      <c r="D7" s="110">
+        <v>106</v>
+      </c>
+      <c r="E7" s="110">
+        <v>210</v>
+      </c>
+      <c r="F7" s="112" t="s">
+        <v>256</v>
+      </c>
+      <c r="G7" s="110">
+        <v>79</v>
+      </c>
+      <c r="H7" s="110">
+        <v>2</v>
+      </c>
+      <c r="I7" s="110">
+        <v>77</v>
+      </c>
+      <c r="J7" s="110">
+        <v>79</v>
+      </c>
+      <c r="K7" s="110">
+        <v>78</v>
+      </c>
+      <c r="L7" s="110">
+        <v>2</v>
+      </c>
+      <c r="M7" s="110">
+        <v>76</v>
+      </c>
+      <c r="N7" s="110">
+        <v>77</v>
+      </c>
+      <c r="O7" s="112" t="s">
+        <v>255</v>
+      </c>
+      <c r="P7" s="110">
+        <v>82</v>
+      </c>
+      <c r="Q7" s="110">
+        <v>8</v>
+      </c>
+      <c r="R7" s="110">
+        <v>74</v>
+      </c>
+      <c r="S7" s="110">
+        <v>81</v>
+      </c>
+      <c r="T7" s="110">
+        <v>83</v>
+      </c>
+      <c r="U7" s="110">
+        <v>8</v>
+      </c>
+      <c r="V7" s="110">
+        <v>75</v>
+      </c>
+      <c r="W7" s="110">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="110">
+        <v>1</v>
+      </c>
+      <c r="B8" s="111" t="s">
+        <v>428</v>
+      </c>
+      <c r="C8" s="110">
+        <v>104</v>
+      </c>
+      <c r="D8" s="110">
+        <v>106</v>
+      </c>
+      <c r="E8" s="110">
+        <v>210</v>
+      </c>
+      <c r="F8" s="112" t="s">
+        <v>294</v>
+      </c>
+      <c r="G8" s="110">
+        <v>83</v>
+      </c>
+      <c r="H8" s="110">
+        <v>10</v>
+      </c>
+      <c r="I8" s="110">
+        <v>73</v>
+      </c>
+      <c r="J8" s="110">
+        <v>83</v>
+      </c>
+      <c r="K8" s="110">
+        <v>80</v>
+      </c>
+      <c r="L8" s="110">
+        <v>10</v>
+      </c>
+      <c r="M8" s="110">
+        <v>70</v>
+      </c>
+      <c r="N8" s="110">
+        <v>80</v>
+      </c>
+      <c r="O8" s="112" t="s">
+        <v>293</v>
+      </c>
+      <c r="P8" s="110">
+        <v>90</v>
+      </c>
+      <c r="Q8" s="110">
+        <v>14</v>
+      </c>
+      <c r="R8" s="110">
+        <v>76</v>
+      </c>
+      <c r="S8" s="110">
+        <v>90</v>
+      </c>
+      <c r="T8" s="110">
+        <v>93</v>
+      </c>
+      <c r="U8" s="110">
+        <v>14</v>
+      </c>
+      <c r="V8" s="110">
+        <v>79</v>
+      </c>
+      <c r="W8" s="110">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="110">
+        <v>1</v>
+      </c>
+      <c r="B9" s="111" t="s">
+        <v>429</v>
+      </c>
+      <c r="C9" s="110">
+        <v>99</v>
+      </c>
+      <c r="D9" s="110">
+        <v>112</v>
+      </c>
+      <c r="E9" s="110">
+        <v>211</v>
+      </c>
+      <c r="F9" s="112" t="s">
+        <v>276</v>
+      </c>
+      <c r="G9" s="110">
+        <v>73</v>
+      </c>
+      <c r="H9" s="110">
+        <v>3</v>
+      </c>
+      <c r="I9" s="110">
+        <v>70</v>
+      </c>
+      <c r="J9" s="110">
+        <v>73</v>
+      </c>
+      <c r="K9" s="110">
+        <v>83</v>
+      </c>
+      <c r="L9" s="110">
+        <v>3</v>
+      </c>
+      <c r="M9" s="110">
+        <v>80</v>
+      </c>
+      <c r="N9" s="110">
+        <v>82</v>
+      </c>
+      <c r="O9" s="112" t="s">
+        <v>275</v>
+      </c>
+      <c r="P9" s="110">
+        <v>73</v>
+      </c>
+      <c r="Q9" s="110">
+        <v>0</v>
+      </c>
+      <c r="R9" s="110">
+        <v>73</v>
+      </c>
+      <c r="S9" s="110">
+        <v>73</v>
+      </c>
+      <c r="T9" s="110">
+        <v>75</v>
+      </c>
+      <c r="U9" s="110">
+        <v>0</v>
+      </c>
+      <c r="V9" s="110">
+        <v>75</v>
+      </c>
+      <c r="W9" s="110">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="110">
+        <v>1</v>
+      </c>
+      <c r="B10" s="111" t="s">
+        <v>430</v>
+      </c>
+      <c r="C10" s="110">
+        <v>105</v>
+      </c>
+      <c r="D10" s="110">
+        <v>109</v>
+      </c>
+      <c r="E10" s="110">
+        <v>214</v>
+      </c>
+      <c r="F10" s="112" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="110">
+        <v>81</v>
+      </c>
+      <c r="H10" s="110">
+        <v>6</v>
+      </c>
+      <c r="I10" s="110">
+        <v>75</v>
+      </c>
+      <c r="J10" s="110">
+        <v>81</v>
+      </c>
+      <c r="K10" s="110">
+        <v>81</v>
+      </c>
+      <c r="L10" s="110">
+        <v>6</v>
+      </c>
+      <c r="M10" s="110">
+        <v>75</v>
+      </c>
+      <c r="N10" s="110">
+        <v>81</v>
+      </c>
+      <c r="O10" s="112" t="s">
+        <v>291</v>
+      </c>
+      <c r="P10" s="110">
+        <v>91</v>
+      </c>
+      <c r="Q10" s="110">
+        <v>12</v>
+      </c>
+      <c r="R10" s="110">
+        <v>79</v>
+      </c>
+      <c r="S10" s="110">
+        <v>89</v>
+      </c>
+      <c r="T10" s="110">
+        <v>88</v>
+      </c>
+      <c r="U10" s="110">
+        <v>12</v>
+      </c>
+      <c r="V10" s="110">
+        <v>76</v>
+      </c>
+      <c r="W10" s="110">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="110">
+        <v>1</v>
+      </c>
+      <c r="B11" s="111" t="s">
+        <v>431</v>
+      </c>
+      <c r="C11" s="110">
+        <v>110</v>
+      </c>
+      <c r="D11" s="110">
+        <v>112</v>
+      </c>
+      <c r="E11" s="110">
+        <v>222</v>
+      </c>
+      <c r="F11" s="112" t="s">
+        <v>268</v>
+      </c>
+      <c r="G11" s="110">
+        <v>78</v>
+      </c>
+      <c r="H11" s="110">
+        <v>6</v>
+      </c>
+      <c r="I11" s="110">
+        <v>72</v>
+      </c>
+      <c r="J11" s="110">
+        <v>78</v>
+      </c>
+      <c r="K11" s="110">
+        <v>77</v>
+      </c>
+      <c r="L11" s="110">
+        <v>6</v>
+      </c>
+      <c r="M11" s="110">
+        <v>71</v>
+      </c>
+      <c r="N11" s="110">
+        <v>77</v>
+      </c>
+      <c r="O11" s="112" t="s">
+        <v>269</v>
+      </c>
+      <c r="P11" s="110">
+        <v>90</v>
+      </c>
+      <c r="Q11" s="110">
+        <v>10</v>
+      </c>
+      <c r="R11" s="110">
+        <v>80</v>
+      </c>
+      <c r="S11" s="110">
+        <v>89</v>
+      </c>
+      <c r="T11" s="110">
+        <v>93</v>
+      </c>
+      <c r="U11" s="110">
+        <v>10</v>
+      </c>
+      <c r="V11" s="110">
+        <v>83</v>
+      </c>
+      <c r="W11" s="110">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="110">
+        <v>1</v>
+      </c>
+      <c r="B12" s="111" t="s">
+        <v>432</v>
+      </c>
+      <c r="C12" s="110">
+        <v>112</v>
+      </c>
+      <c r="D12" s="110">
+        <v>110</v>
+      </c>
+      <c r="E12" s="110">
+        <v>222</v>
+      </c>
+      <c r="F12" s="112" t="s">
+        <v>433</v>
+      </c>
+      <c r="G12" s="110">
+        <v>78</v>
+      </c>
+      <c r="H12" s="110">
+        <v>5</v>
+      </c>
+      <c r="I12" s="110">
+        <v>73</v>
+      </c>
+      <c r="J12" s="110">
+        <v>78</v>
+      </c>
+      <c r="K12" s="110">
+        <v>83</v>
+      </c>
+      <c r="L12" s="110">
+        <v>5</v>
+      </c>
+      <c r="M12" s="110">
+        <v>78</v>
+      </c>
+      <c r="N12" s="110">
+        <v>83</v>
+      </c>
+      <c r="O12" s="112" t="s">
+        <v>257</v>
+      </c>
+      <c r="P12" s="110">
+        <v>86</v>
+      </c>
+      <c r="Q12" s="110">
+        <v>2</v>
+      </c>
+      <c r="R12" s="110">
+        <v>84</v>
+      </c>
+      <c r="S12" s="110">
+        <v>83</v>
+      </c>
+      <c r="T12" s="110">
+        <v>80</v>
+      </c>
+      <c r="U12" s="110">
+        <v>2</v>
+      </c>
+      <c r="V12" s="110">
+        <v>78</v>
+      </c>
+      <c r="W12" s="110">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="113">
+        <v>2</v>
+      </c>
+      <c r="B13" s="114" t="s">
+        <v>434</v>
+      </c>
+      <c r="C13" s="113">
+        <v>90</v>
+      </c>
+      <c r="D13" s="113">
+        <v>103</v>
+      </c>
+      <c r="E13" s="113">
+        <v>193</v>
+      </c>
+      <c r="F13" s="115" t="s">
+        <v>266</v>
+      </c>
+      <c r="G13" s="113">
+        <v>87</v>
+      </c>
+      <c r="H13" s="113">
+        <v>22</v>
+      </c>
+      <c r="I13" s="113">
+        <v>65</v>
+      </c>
+      <c r="J13" s="113">
+        <v>87</v>
+      </c>
+      <c r="K13" s="113">
+        <v>92</v>
+      </c>
+      <c r="L13" s="113">
+        <v>22</v>
+      </c>
+      <c r="M13" s="113">
+        <v>70</v>
+      </c>
+      <c r="N13" s="113">
+        <v>92</v>
+      </c>
+      <c r="O13" s="115" t="s">
+        <v>267</v>
+      </c>
+      <c r="P13" s="113">
+        <v>85</v>
+      </c>
+      <c r="Q13" s="113">
+        <v>13</v>
+      </c>
+      <c r="R13" s="113">
+        <v>72</v>
+      </c>
+      <c r="S13" s="113">
+        <v>85</v>
+      </c>
+      <c r="T13" s="113">
+        <v>87</v>
+      </c>
+      <c r="U13" s="113">
+        <v>13</v>
+      </c>
+      <c r="V13" s="113">
+        <v>74</v>
+      </c>
+      <c r="W13" s="113">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="113">
+        <v>2</v>
+      </c>
+      <c r="B14" s="114" t="s">
+        <v>435</v>
+      </c>
+      <c r="C14" s="113">
+        <v>104</v>
+      </c>
+      <c r="D14" s="113">
+        <v>104</v>
+      </c>
+      <c r="E14" s="113">
+        <v>208</v>
+      </c>
+      <c r="F14" s="115" t="s">
+        <v>286</v>
+      </c>
+      <c r="G14" s="113">
+        <v>100</v>
+      </c>
+      <c r="H14" s="113">
+        <v>18</v>
+      </c>
+      <c r="I14" s="113">
+        <v>82</v>
+      </c>
+      <c r="J14" s="113">
+        <v>99</v>
+      </c>
+      <c r="K14" s="113">
+        <v>93</v>
+      </c>
+      <c r="L14" s="113">
+        <v>18</v>
+      </c>
+      <c r="M14" s="113">
+        <v>75</v>
+      </c>
+      <c r="N14" s="113">
+        <v>93</v>
+      </c>
+      <c r="O14" s="115" t="s">
+        <v>285</v>
+      </c>
+      <c r="P14" s="113">
+        <v>77</v>
+      </c>
+      <c r="Q14" s="113">
+        <v>11</v>
+      </c>
+      <c r="R14" s="113">
+        <v>66</v>
+      </c>
+      <c r="S14" s="113">
+        <v>77</v>
+      </c>
+      <c r="T14" s="113">
+        <v>85</v>
+      </c>
+      <c r="U14" s="113">
+        <v>11</v>
+      </c>
+      <c r="V14" s="113">
+        <v>74</v>
+      </c>
+      <c r="W14" s="113">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="113">
+        <v>2</v>
+      </c>
+      <c r="B15" s="114" t="s">
+        <v>436</v>
+      </c>
+      <c r="C15" s="113">
+        <v>102</v>
+      </c>
+      <c r="D15" s="113">
+        <v>109</v>
+      </c>
+      <c r="E15" s="113">
+        <v>211</v>
+      </c>
+      <c r="F15" s="115" t="s">
+        <v>299</v>
+      </c>
+      <c r="G15" s="113">
+        <v>93</v>
+      </c>
+      <c r="H15" s="113">
+        <v>18</v>
+      </c>
+      <c r="I15" s="113">
+        <v>75</v>
+      </c>
+      <c r="J15" s="113">
+        <v>91</v>
+      </c>
+      <c r="K15" s="113">
+        <v>92</v>
+      </c>
+      <c r="L15" s="113">
+        <v>18</v>
+      </c>
+      <c r="M15" s="113">
+        <v>74</v>
+      </c>
+      <c r="N15" s="113">
+        <v>91</v>
+      </c>
+      <c r="O15" s="115" t="s">
+        <v>300</v>
+      </c>
+      <c r="P15" s="113">
+        <v>87</v>
+      </c>
+      <c r="Q15" s="113">
+        <v>14</v>
+      </c>
+      <c r="R15" s="113">
+        <v>73</v>
+      </c>
+      <c r="S15" s="113">
+        <v>87</v>
+      </c>
+      <c r="T15" s="113">
+        <v>95</v>
+      </c>
+      <c r="U15" s="113">
+        <v>14</v>
+      </c>
+      <c r="V15" s="113">
+        <v>81</v>
+      </c>
+      <c r="W15" s="113">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="113">
+        <v>2</v>
+      </c>
+      <c r="B16" s="114" t="s">
+        <v>437</v>
+      </c>
+      <c r="C16" s="113">
+        <v>104</v>
+      </c>
+      <c r="D16" s="113">
+        <v>107</v>
+      </c>
+      <c r="E16" s="113">
+        <v>211</v>
+      </c>
+      <c r="F16" s="115" t="s">
+        <v>265</v>
+      </c>
+      <c r="G16" s="113">
+        <v>81</v>
+      </c>
+      <c r="H16" s="113">
+        <v>8</v>
+      </c>
+      <c r="I16" s="113">
+        <v>73</v>
+      </c>
+      <c r="J16" s="113">
+        <v>81</v>
+      </c>
+      <c r="K16" s="113">
+        <v>79</v>
+      </c>
+      <c r="L16" s="113">
+        <v>8</v>
+      </c>
+      <c r="M16" s="113">
+        <v>71</v>
+      </c>
+      <c r="N16" s="113">
+        <v>79</v>
+      </c>
+      <c r="O16" s="115" t="s">
+        <v>270</v>
+      </c>
+      <c r="P16" s="113">
+        <v>103</v>
+      </c>
+      <c r="Q16" s="113">
+        <v>20</v>
+      </c>
+      <c r="R16" s="113">
+        <v>83</v>
+      </c>
+      <c r="S16" s="113">
+        <v>103</v>
+      </c>
+      <c r="T16" s="113">
+        <v>94</v>
+      </c>
+      <c r="U16" s="113">
+        <v>20</v>
+      </c>
+      <c r="V16" s="113">
+        <v>74</v>
+      </c>
+      <c r="W16" s="113">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17" s="113">
+        <v>2</v>
+      </c>
+      <c r="B17" s="114" t="s">
+        <v>439</v>
+      </c>
+      <c r="C17" s="113">
+        <v>104</v>
+      </c>
+      <c r="D17" s="113">
+        <v>111</v>
+      </c>
+      <c r="E17" s="113">
+        <v>215</v>
+      </c>
+      <c r="F17" s="115" t="s">
+        <v>290</v>
+      </c>
+      <c r="G17" s="113">
+        <v>100</v>
+      </c>
+      <c r="H17" s="113">
+        <v>22</v>
+      </c>
+      <c r="I17" s="113">
+        <v>78</v>
+      </c>
+      <c r="J17" s="113">
+        <v>100</v>
+      </c>
+      <c r="K17" s="113">
+        <v>102</v>
+      </c>
+      <c r="L17" s="113">
+        <v>22</v>
+      </c>
+      <c r="M17" s="113">
+        <v>80</v>
+      </c>
+      <c r="N17" s="113">
+        <v>102</v>
+      </c>
+      <c r="O17" s="115" t="s">
+        <v>289</v>
+      </c>
+      <c r="P17" s="113">
+        <v>89</v>
+      </c>
+      <c r="Q17" s="113">
+        <v>12</v>
+      </c>
+      <c r="R17" s="113">
+        <v>77</v>
+      </c>
+      <c r="S17" s="113">
+        <v>89</v>
+      </c>
+      <c r="T17" s="113">
+        <v>85</v>
+      </c>
+      <c r="U17" s="113">
+        <v>12</v>
+      </c>
+      <c r="V17" s="113">
+        <v>73</v>
+      </c>
+      <c r="W17" s="113">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A18" s="113">
+        <v>2</v>
+      </c>
+      <c r="B18" s="114" t="s">
+        <v>440</v>
+      </c>
+      <c r="C18" s="113">
+        <v>107</v>
+      </c>
+      <c r="D18" s="113">
+        <v>108</v>
+      </c>
+      <c r="E18" s="113">
+        <v>215</v>
+      </c>
+      <c r="F18" s="115" t="s">
+        <v>298</v>
+      </c>
+      <c r="G18" s="113">
+        <v>98</v>
+      </c>
+      <c r="H18" s="113">
+        <v>18</v>
+      </c>
+      <c r="I18" s="113">
+        <v>80</v>
+      </c>
+      <c r="J18" s="113">
+        <v>94</v>
+      </c>
+      <c r="K18" s="113">
+        <v>88</v>
+      </c>
+      <c r="L18" s="113">
+        <v>18</v>
+      </c>
+      <c r="M18" s="113">
+        <v>70</v>
+      </c>
+      <c r="N18" s="113">
+        <v>88</v>
+      </c>
+      <c r="O18" s="115" t="s">
+        <v>297</v>
+      </c>
+      <c r="P18" s="113">
+        <v>85</v>
+      </c>
+      <c r="Q18" s="113">
+        <v>11</v>
+      </c>
+      <c r="R18" s="113">
+        <v>74</v>
+      </c>
+      <c r="S18" s="113">
+        <v>85</v>
+      </c>
+      <c r="T18" s="113">
+        <v>89</v>
+      </c>
+      <c r="U18" s="113">
+        <v>11</v>
+      </c>
+      <c r="V18" s="113">
+        <v>78</v>
+      </c>
+      <c r="W18" s="113">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A19" s="113">
+        <v>2</v>
+      </c>
+      <c r="B19" s="114" t="s">
+        <v>438</v>
+      </c>
+      <c r="C19" s="113">
+        <v>102</v>
+      </c>
+      <c r="D19" s="113">
+        <v>113</v>
+      </c>
+      <c r="E19" s="113">
+        <v>215</v>
+      </c>
+      <c r="F19" s="115" t="s">
+        <v>357</v>
+      </c>
+      <c r="G19" s="113">
+        <v>93</v>
+      </c>
+      <c r="H19" s="113">
+        <v>12</v>
+      </c>
+      <c r="I19" s="113">
+        <v>81</v>
+      </c>
+      <c r="J19" s="113">
+        <v>91</v>
+      </c>
+      <c r="K19" s="113">
+        <v>96</v>
+      </c>
+      <c r="L19" s="113">
+        <v>12</v>
+      </c>
+      <c r="M19" s="113">
+        <v>84</v>
+      </c>
+      <c r="N19" s="113">
+        <v>95</v>
+      </c>
+      <c r="O19" s="115" t="s">
+        <v>356</v>
+      </c>
+      <c r="P19" s="113">
+        <v>81</v>
+      </c>
+      <c r="Q19" s="113">
+        <v>15</v>
+      </c>
+      <c r="R19" s="113">
+        <v>66</v>
+      </c>
+      <c r="S19" s="113">
+        <v>81</v>
+      </c>
+      <c r="T19" s="113">
+        <v>85</v>
+      </c>
+      <c r="U19" s="113">
+        <v>15</v>
+      </c>
+      <c r="V19" s="113">
+        <v>70</v>
+      </c>
+      <c r="W19" s="113">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A20" s="113">
+        <v>2</v>
+      </c>
+      <c r="B20" s="114" t="s">
+        <v>441</v>
+      </c>
+      <c r="C20" s="113">
+        <v>103</v>
+      </c>
+      <c r="D20" s="113">
+        <v>113</v>
+      </c>
+      <c r="E20" s="113">
+        <v>216</v>
+      </c>
+      <c r="F20" s="115" t="s">
+        <v>342</v>
+      </c>
+      <c r="G20" s="113">
+        <v>86</v>
+      </c>
+      <c r="H20" s="113">
+        <v>8</v>
+      </c>
+      <c r="I20" s="113">
+        <v>78</v>
+      </c>
+      <c r="J20" s="113">
+        <v>83</v>
+      </c>
+      <c r="K20" s="113">
+        <v>84</v>
+      </c>
+      <c r="L20" s="113">
+        <v>8</v>
+      </c>
+      <c r="M20" s="113">
+        <v>76</v>
+      </c>
+      <c r="N20" s="113">
+        <v>84</v>
+      </c>
+      <c r="O20" s="115" t="s">
+        <v>340</v>
+      </c>
+      <c r="P20" s="113">
+        <v>90</v>
+      </c>
+      <c r="Q20" s="113">
+        <v>20</v>
+      </c>
+      <c r="R20" s="113">
+        <v>70</v>
+      </c>
+      <c r="S20" s="113">
+        <v>89</v>
+      </c>
+      <c r="T20" s="113">
+        <v>104</v>
+      </c>
+      <c r="U20" s="113">
+        <v>20</v>
+      </c>
+      <c r="V20" s="113">
+        <v>84</v>
+      </c>
+      <c r="W20" s="113">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A21" s="113">
+        <v>2</v>
+      </c>
+      <c r="B21" s="114" t="s">
+        <v>442</v>
+      </c>
+      <c r="C21" s="113">
+        <v>106</v>
+      </c>
+      <c r="D21" s="113">
+        <v>122</v>
+      </c>
+      <c r="E21" s="113">
+        <v>228</v>
+      </c>
+      <c r="F21" s="115" t="s">
+        <v>282</v>
+      </c>
+      <c r="G21" s="113">
+        <v>90</v>
+      </c>
+      <c r="H21" s="113">
+        <v>13</v>
+      </c>
+      <c r="I21" s="113">
+        <v>77</v>
+      </c>
+      <c r="J21" s="113">
+        <v>89</v>
+      </c>
+      <c r="K21" s="113">
+        <v>93</v>
+      </c>
+      <c r="L21" s="113">
+        <v>13</v>
+      </c>
+      <c r="M21" s="113">
+        <v>80</v>
+      </c>
+      <c r="N21" s="113">
+        <v>92</v>
+      </c>
+      <c r="O21" s="115" t="s">
+        <v>281</v>
+      </c>
+      <c r="P21" s="113">
+        <v>91</v>
+      </c>
+      <c r="Q21" s="113">
+        <v>13</v>
+      </c>
+      <c r="R21" s="113">
+        <v>78</v>
+      </c>
+      <c r="S21" s="113">
+        <v>91</v>
+      </c>
+      <c r="T21" s="113">
+        <v>96</v>
+      </c>
+      <c r="U21" s="113">
+        <v>13</v>
+      </c>
+      <c r="V21" s="113">
+        <v>83</v>
+      </c>
+      <c r="W21" s="113">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A22" s="113">
+        <v>2</v>
+      </c>
+      <c r="B22" s="114" t="s">
+        <v>443</v>
+      </c>
+      <c r="C22" s="113">
+        <v>126</v>
+      </c>
+      <c r="D22" s="113">
+        <v>110</v>
+      </c>
+      <c r="E22" s="113">
+        <v>236</v>
+      </c>
+      <c r="F22" s="115" t="s">
+        <v>283</v>
+      </c>
+      <c r="G22" s="113">
+        <v>104</v>
+      </c>
+      <c r="H22" s="113">
+        <v>12</v>
+      </c>
+      <c r="I22" s="113">
+        <v>92</v>
+      </c>
+      <c r="J22" s="113">
+        <v>101</v>
+      </c>
+      <c r="K22" s="113">
+        <v>85</v>
+      </c>
+      <c r="L22" s="113">
+        <v>12</v>
+      </c>
+      <c r="M22" s="113">
+        <v>73</v>
+      </c>
+      <c r="N22" s="113">
+        <v>84</v>
+      </c>
+      <c r="O22" s="115" t="s">
+        <v>284</v>
+      </c>
+      <c r="P22" s="113">
+        <v>97</v>
+      </c>
+      <c r="Q22" s="113">
+        <v>13</v>
+      </c>
+      <c r="R22" s="113">
+        <v>84</v>
+      </c>
+      <c r="S22" s="113">
+        <v>95</v>
+      </c>
+      <c r="T22" s="113">
+        <v>90</v>
+      </c>
+      <c r="U22" s="113">
+        <v>13</v>
+      </c>
+      <c r="V22" s="113">
+        <v>77</v>
+      </c>
+      <c r="W22" s="113">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23" s="113">
+        <v>2</v>
+      </c>
+      <c r="B23" s="114" t="s">
+        <v>444</v>
+      </c>
+      <c r="C23" s="113">
+        <v>111</v>
+      </c>
+      <c r="D23" s="113">
+        <v>130</v>
+      </c>
+      <c r="E23" s="113">
+        <v>241</v>
+      </c>
+      <c r="F23" s="115" t="s">
+        <v>280</v>
+      </c>
+      <c r="G23" s="113">
+        <v>93</v>
+      </c>
+      <c r="H23" s="113">
+        <v>17</v>
+      </c>
+      <c r="I23" s="113">
+        <v>76</v>
+      </c>
+      <c r="J23" s="113">
+        <v>92</v>
+      </c>
+      <c r="K23" s="113">
+        <v>93</v>
+      </c>
+      <c r="L23" s="113">
+        <v>17</v>
+      </c>
+      <c r="M23" s="113">
+        <v>76</v>
+      </c>
+      <c r="N23" s="113">
+        <v>93</v>
+      </c>
+      <c r="O23" s="115" t="s">
+        <v>279</v>
+      </c>
+      <c r="P23" s="113">
+        <v>101</v>
+      </c>
+      <c r="Q23" s="113">
+        <v>15</v>
+      </c>
+      <c r="R23" s="113">
+        <v>86</v>
+      </c>
+      <c r="S23" s="113">
+        <v>99</v>
+      </c>
+      <c r="T23" s="113">
+        <v>115</v>
+      </c>
+      <c r="U23" s="113">
+        <v>15</v>
+      </c>
+      <c r="V23" s="113">
+        <v>100</v>
+      </c>
+      <c r="W23" s="113">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A24" s="116">
+        <v>3</v>
+      </c>
+      <c r="B24" s="117" t="s">
+        <v>445</v>
+      </c>
+      <c r="C24" s="116">
+        <v>103</v>
+      </c>
+      <c r="D24" s="116">
+        <v>96</v>
+      </c>
+      <c r="E24" s="116">
+        <v>199</v>
+      </c>
+      <c r="F24" s="118" t="s">
+        <v>287</v>
+      </c>
+      <c r="G24" s="116">
+        <v>98</v>
+      </c>
+      <c r="H24" s="116">
+        <v>23</v>
+      </c>
+      <c r="I24" s="116">
+        <v>75</v>
+      </c>
+      <c r="J24" s="116">
+        <v>98</v>
+      </c>
+      <c r="K24" s="116">
+        <v>96</v>
+      </c>
+      <c r="L24" s="116">
+        <v>23</v>
+      </c>
+      <c r="M24" s="116">
+        <v>73</v>
+      </c>
+      <c r="N24" s="116">
+        <v>96</v>
+      </c>
+      <c r="O24" s="118" t="s">
+        <v>288</v>
+      </c>
+      <c r="P24" s="116">
+        <v>93</v>
+      </c>
+      <c r="Q24" s="116">
+        <v>19</v>
+      </c>
+      <c r="R24" s="116">
+        <v>74</v>
+      </c>
+      <c r="S24" s="116">
+        <v>92</v>
+      </c>
+      <c r="T24" s="116">
+        <v>89</v>
+      </c>
+      <c r="U24" s="116">
+        <v>19</v>
+      </c>
+      <c r="V24" s="116">
+        <v>70</v>
+      </c>
+      <c r="W24" s="116">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A25" s="116">
+        <v>3</v>
+      </c>
+      <c r="B25" s="117" t="s">
+        <v>446</v>
+      </c>
+      <c r="C25" s="116">
+        <v>101</v>
+      </c>
+      <c r="D25" s="116">
+        <v>102</v>
+      </c>
+      <c r="E25" s="116">
+        <v>203</v>
+      </c>
+      <c r="F25" s="118" t="s">
+        <v>271</v>
+      </c>
+      <c r="G25" s="116">
+        <v>100</v>
+      </c>
+      <c r="H25" s="116">
+        <v>22</v>
+      </c>
+      <c r="I25" s="116">
+        <v>78</v>
+      </c>
+      <c r="J25" s="116">
+        <v>100</v>
+      </c>
+      <c r="K25" s="116">
+        <v>93</v>
+      </c>
+      <c r="L25" s="116">
+        <v>22</v>
+      </c>
+      <c r="M25" s="116">
+        <v>71</v>
+      </c>
+      <c r="N25" s="116">
+        <v>93</v>
+      </c>
+      <c r="O25" s="118" t="s">
+        <v>272</v>
+      </c>
+      <c r="P25" s="116">
+        <v>100</v>
+      </c>
+      <c r="Q25" s="116">
+        <v>24</v>
+      </c>
+      <c r="R25" s="116">
+        <v>76</v>
+      </c>
+      <c r="S25" s="116">
+        <v>100</v>
+      </c>
+      <c r="T25" s="116">
+        <v>99</v>
+      </c>
+      <c r="U25" s="116">
+        <v>24</v>
+      </c>
+      <c r="V25" s="116">
+        <v>75</v>
+      </c>
+      <c r="W25" s="116">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A26" s="116">
+        <v>3</v>
+      </c>
+      <c r="B26" s="117" t="s">
+        <v>447</v>
+      </c>
+      <c r="C26" s="116">
+        <v>105</v>
+      </c>
+      <c r="D26" s="116">
+        <v>101</v>
+      </c>
+      <c r="E26" s="116">
+        <v>206</v>
+      </c>
+      <c r="F26" s="118" t="s">
+        <v>307</v>
+      </c>
+      <c r="G26" s="116">
+        <v>93</v>
+      </c>
+      <c r="H26" s="116">
+        <v>23</v>
+      </c>
+      <c r="I26" s="116">
+        <v>70</v>
+      </c>
+      <c r="J26" s="116">
+        <v>92</v>
+      </c>
+      <c r="K26" s="116">
+        <v>92</v>
+      </c>
+      <c r="L26" s="116">
+        <v>23</v>
+      </c>
+      <c r="M26" s="116">
+        <v>69</v>
+      </c>
+      <c r="N26" s="116">
+        <v>92</v>
+      </c>
+      <c r="O26" s="118" t="s">
+        <v>308</v>
+      </c>
+      <c r="P26" s="116">
+        <v>115</v>
+      </c>
+      <c r="Q26" s="116">
+        <v>28</v>
+      </c>
+      <c r="R26" s="116">
+        <v>87</v>
+      </c>
+      <c r="S26" s="116">
+        <v>114</v>
+      </c>
+      <c r="T26" s="116">
+        <v>103</v>
+      </c>
+      <c r="U26" s="116">
+        <v>28</v>
+      </c>
+      <c r="V26" s="116">
+        <v>75</v>
+      </c>
+      <c r="W26" s="116">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A27" s="116">
+        <v>3</v>
+      </c>
+      <c r="B27" s="117" t="s">
+        <v>448</v>
+      </c>
+      <c r="C27" s="116">
+        <v>104</v>
+      </c>
+      <c r="D27" s="116">
+        <v>106</v>
+      </c>
+      <c r="E27" s="116">
+        <v>210</v>
+      </c>
+      <c r="F27" s="118" t="s">
+        <v>302</v>
+      </c>
+      <c r="G27" s="116">
+        <v>83</v>
+      </c>
+      <c r="H27" s="116">
+        <v>14</v>
+      </c>
+      <c r="I27" s="116">
+        <v>69</v>
+      </c>
+      <c r="J27" s="116">
+        <v>82</v>
+      </c>
+      <c r="K27" s="116">
+        <v>92</v>
+      </c>
+      <c r="L27" s="116">
+        <v>14</v>
+      </c>
+      <c r="M27" s="116">
+        <v>78</v>
+      </c>
+      <c r="N27" s="116">
+        <v>91</v>
+      </c>
+      <c r="O27" s="118" t="s">
+        <v>301</v>
+      </c>
+      <c r="P27" s="116">
+        <v>102</v>
+      </c>
+      <c r="Q27" s="116">
+        <v>21</v>
+      </c>
+      <c r="R27" s="116">
+        <v>81</v>
+      </c>
+      <c r="S27" s="116">
+        <v>102</v>
+      </c>
+      <c r="T27" s="116">
+        <v>92</v>
+      </c>
+      <c r="U27" s="116">
+        <v>21</v>
+      </c>
+      <c r="V27" s="116">
+        <v>71</v>
+      </c>
+      <c r="W27" s="116">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A28" s="116">
+        <v>3</v>
+      </c>
+      <c r="B28" s="117" t="s">
+        <v>449</v>
+      </c>
+      <c r="C28" s="116">
+        <v>100</v>
+      </c>
+      <c r="D28" s="116">
+        <v>112</v>
+      </c>
+      <c r="E28" s="116">
+        <v>212</v>
+      </c>
+      <c r="F28" s="118" t="s">
+        <v>296</v>
+      </c>
+      <c r="G28" s="116">
+        <v>109</v>
+      </c>
+      <c r="H28" s="116">
+        <v>35</v>
+      </c>
+      <c r="I28" s="116">
+        <v>74</v>
+      </c>
+      <c r="J28" s="116">
+        <v>108</v>
+      </c>
+      <c r="K28" s="116">
+        <v>111</v>
+      </c>
+      <c r="L28" s="116">
+        <v>35</v>
+      </c>
+      <c r="M28" s="116">
+        <v>76</v>
+      </c>
+      <c r="N28" s="116">
+        <v>111</v>
+      </c>
+      <c r="O28" s="118" t="s">
+        <v>295</v>
+      </c>
+      <c r="P28" s="116">
+        <v>91</v>
+      </c>
+      <c r="Q28" s="116">
+        <v>19</v>
+      </c>
+      <c r="R28" s="116">
+        <v>72</v>
+      </c>
+      <c r="S28" s="116">
+        <v>91</v>
+      </c>
+      <c r="T28" s="116">
+        <v>93</v>
+      </c>
+      <c r="U28" s="116">
+        <v>19</v>
+      </c>
+      <c r="V28" s="116">
+        <v>74</v>
+      </c>
+      <c r="W28" s="116">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A29" s="116">
+        <v>3</v>
+      </c>
+      <c r="B29" s="117" t="s">
+        <v>450</v>
+      </c>
+      <c r="C29" s="116">
+        <v>104</v>
+      </c>
+      <c r="D29" s="116">
+        <v>108</v>
+      </c>
+      <c r="E29" s="116">
+        <v>212</v>
+      </c>
+      <c r="F29" s="118" t="s">
+        <v>135</v>
+      </c>
+      <c r="G29" s="116">
+        <v>110</v>
+      </c>
+      <c r="H29" s="116">
+        <v>40</v>
+      </c>
+      <c r="I29" s="116">
+        <v>70</v>
+      </c>
+      <c r="J29" s="116">
+        <v>110</v>
+      </c>
+      <c r="K29" s="116">
+        <v>118</v>
+      </c>
+      <c r="L29" s="116">
+        <v>40</v>
+      </c>
+      <c r="M29" s="116">
+        <v>78</v>
+      </c>
+      <c r="N29" s="116">
+        <v>118</v>
+      </c>
+      <c r="O29" s="118" t="s">
+        <v>134</v>
+      </c>
+      <c r="P29" s="116">
+        <v>120</v>
+      </c>
+      <c r="Q29" s="116">
+        <v>36</v>
+      </c>
+      <c r="R29" s="116">
+        <v>84</v>
+      </c>
+      <c r="S29" s="116">
+        <v>120</v>
+      </c>
+      <c r="T29" s="116">
+        <v>110</v>
+      </c>
+      <c r="U29" s="116">
+        <v>36</v>
+      </c>
+      <c r="V29" s="116">
+        <v>74</v>
+      </c>
+      <c r="W29" s="116">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A30" s="116">
+        <v>3</v>
+      </c>
+      <c r="B30" s="117" t="s">
+        <v>455</v>
+      </c>
+      <c r="C30" s="116">
+        <v>98</v>
+      </c>
+      <c r="D30" s="116">
+        <v>115</v>
+      </c>
+      <c r="E30" s="116">
+        <v>213</v>
+      </c>
+      <c r="F30" s="118" t="s">
+        <v>309</v>
+      </c>
+      <c r="G30" s="116">
+        <v>85</v>
+      </c>
+      <c r="H30" s="116">
+        <v>21</v>
+      </c>
+      <c r="I30" s="116">
+        <v>64</v>
+      </c>
+      <c r="J30" s="116">
+        <v>85</v>
+      </c>
+      <c r="K30" s="116">
+        <v>95</v>
+      </c>
+      <c r="L30" s="116">
+        <v>21</v>
+      </c>
+      <c r="M30" s="116">
+        <v>74</v>
+      </c>
+      <c r="N30" s="116">
+        <v>94</v>
+      </c>
+      <c r="O30" s="118" t="s">
+        <v>310</v>
+      </c>
+      <c r="P30" s="116">
+        <v>116</v>
+      </c>
+      <c r="Q30" s="116">
+        <v>31</v>
+      </c>
+      <c r="R30" s="116">
+        <v>85</v>
+      </c>
+      <c r="S30" s="116">
+        <v>116</v>
+      </c>
+      <c r="T30" s="116">
+        <v>118</v>
+      </c>
+      <c r="U30" s="116">
+        <v>31</v>
+      </c>
+      <c r="V30" s="116">
+        <v>87</v>
+      </c>
+      <c r="W30" s="116">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A31" s="116">
+        <v>3</v>
+      </c>
+      <c r="B31" s="117" t="s">
+        <v>452</v>
+      </c>
+      <c r="C31" s="116">
+        <v>107</v>
+      </c>
+      <c r="D31" s="116">
+        <v>106</v>
+      </c>
+      <c r="E31" s="116">
+        <v>213</v>
+      </c>
+      <c r="F31" s="118" t="s">
+        <v>311</v>
+      </c>
+      <c r="G31" s="116">
+        <v>102</v>
+      </c>
+      <c r="H31" s="116">
+        <v>25</v>
+      </c>
+      <c r="I31" s="116">
+        <v>77</v>
+      </c>
+      <c r="J31" s="116">
+        <v>100</v>
+      </c>
+      <c r="K31" s="116">
+        <v>101</v>
+      </c>
+      <c r="L31" s="116">
+        <v>25</v>
+      </c>
+      <c r="M31" s="116">
+        <v>76</v>
+      </c>
+      <c r="N31" s="116">
+        <v>101</v>
+      </c>
+      <c r="O31" s="118" t="s">
+        <v>312</v>
+      </c>
+      <c r="P31" s="116">
+        <v>123</v>
+      </c>
+      <c r="Q31" s="116">
+        <v>43</v>
+      </c>
+      <c r="R31" s="116">
+        <v>80</v>
+      </c>
+      <c r="S31" s="116">
+        <v>123</v>
+      </c>
+      <c r="T31" s="116">
+        <v>113</v>
+      </c>
+      <c r="U31" s="116">
+        <v>43</v>
+      </c>
+      <c r="V31" s="116">
+        <v>70</v>
+      </c>
+      <c r="W31" s="116">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A32" s="116">
+        <v>3</v>
+      </c>
+      <c r="B32" s="117" t="s">
+        <v>451</v>
+      </c>
+      <c r="C32" s="116">
+        <v>103</v>
+      </c>
+      <c r="D32" s="116">
+        <v>111</v>
+      </c>
+      <c r="E32" s="116">
+        <v>214</v>
+      </c>
+      <c r="F32" s="118" t="s">
+        <v>305</v>
+      </c>
+      <c r="G32" s="116">
+        <v>88</v>
+      </c>
+      <c r="H32" s="116">
+        <v>15</v>
+      </c>
+      <c r="I32" s="116">
+        <v>73</v>
+      </c>
+      <c r="J32" s="116">
+        <v>88</v>
+      </c>
+      <c r="K32" s="116">
+        <v>87</v>
+      </c>
+      <c r="L32" s="116">
+        <v>15</v>
+      </c>
+      <c r="M32" s="116">
+        <v>72</v>
+      </c>
+      <c r="N32" s="116">
+        <v>87</v>
+      </c>
+      <c r="O32" s="118" t="s">
+        <v>306</v>
+      </c>
+      <c r="P32" s="116">
+        <v>104</v>
+      </c>
+      <c r="Q32" s="116">
+        <v>27</v>
+      </c>
+      <c r="R32" s="116">
+        <v>77</v>
+      </c>
+      <c r="S32" s="116">
+        <v>103</v>
+      </c>
+      <c r="T32" s="116">
+        <v>107</v>
+      </c>
+      <c r="U32" s="116">
+        <v>27</v>
+      </c>
+      <c r="V32" s="116">
+        <v>80</v>
+      </c>
+      <c r="W32" s="116">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A33" s="116">
+        <v>3</v>
+      </c>
+      <c r="B33" s="117" t="s">
+        <v>453</v>
+      </c>
+      <c r="C33" s="116">
+        <v>103</v>
+      </c>
+      <c r="D33" s="116">
+        <v>115</v>
+      </c>
+      <c r="E33" s="116">
+        <v>218</v>
+      </c>
+      <c r="F33" s="118" t="s">
+        <v>273</v>
+      </c>
+      <c r="G33" s="116">
+        <v>88</v>
+      </c>
+      <c r="H33" s="116">
+        <v>10</v>
+      </c>
+      <c r="I33" s="116">
+        <v>78</v>
+      </c>
+      <c r="J33" s="116">
+        <v>88</v>
+      </c>
+      <c r="K33" s="116">
+        <v>88</v>
+      </c>
+      <c r="L33" s="116">
+        <v>10</v>
+      </c>
+      <c r="M33" s="116">
+        <v>78</v>
+      </c>
+      <c r="N33" s="116">
+        <v>86</v>
+      </c>
+      <c r="O33" s="118" t="s">
+        <v>274</v>
+      </c>
+      <c r="P33" s="116">
+        <v>100</v>
+      </c>
+      <c r="Q33" s="116">
+        <v>28</v>
+      </c>
+      <c r="R33" s="116">
+        <v>72</v>
+      </c>
+      <c r="S33" s="116">
+        <v>100</v>
+      </c>
+      <c r="T33" s="116">
+        <v>112</v>
+      </c>
+      <c r="U33" s="116">
+        <v>28</v>
+      </c>
+      <c r="V33" s="116">
+        <v>84</v>
+      </c>
+      <c r="W33" s="116">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A34" s="116">
+        <v>3</v>
+      </c>
+      <c r="B34" s="117" t="s">
+        <v>454</v>
+      </c>
+      <c r="C34" s="116">
+        <v>110</v>
+      </c>
+      <c r="D34" s="116">
+        <v>113</v>
+      </c>
+      <c r="E34" s="116">
+        <v>223</v>
+      </c>
+      <c r="F34" s="118" t="s">
+        <v>303</v>
+      </c>
+      <c r="G34" s="116">
+        <v>114</v>
+      </c>
+      <c r="H34" s="116">
+        <v>30</v>
+      </c>
+      <c r="I34" s="116">
+        <v>84</v>
+      </c>
+      <c r="J34" s="116">
+        <v>114</v>
+      </c>
+      <c r="K34" s="116">
+        <v>114</v>
+      </c>
+      <c r="L34" s="116">
+        <v>30</v>
+      </c>
+      <c r="M34" s="116">
+        <v>84</v>
+      </c>
+      <c r="N34" s="116">
+        <v>114</v>
+      </c>
+      <c r="O34" s="118" t="s">
+        <v>304</v>
+      </c>
+      <c r="P34" s="116">
+        <v>85</v>
+      </c>
+      <c r="Q34" s="116">
+        <v>9</v>
+      </c>
+      <c r="R34" s="116">
+        <v>76</v>
+      </c>
+      <c r="S34" s="116">
+        <v>85</v>
+      </c>
+      <c r="T34" s="116">
+        <v>88</v>
+      </c>
+      <c r="U34" s="116">
+        <v>9</v>
+      </c>
+      <c r="V34" s="116">
+        <v>79</v>
+      </c>
+      <c r="W34" s="116">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>